<commit_message>
FIX: Tipos de cambio CORREGIDOS con valores reales
CORRECCIÓN CRÍTICA:
❌ ANTES (inventados):
   TC Compra: ₡517.50
   TC Venta: ₡525.00

✅ AHORA (reales 12/Nov/2025):
   TC Compra: ₡494.00
   TC Venta: ₡508.00

IMPACTO EN FÓRMULAS:
1. EFECTIVO - TOTAL BANCOS:
   - Conversión CRC→USD usa ₡494.00
   - Fórmula: SUMIF CRC / 494

2. TARJETAS - Equivalente USD:
   - MC 8759 (₡863,830) ahora = $1,748.44
   - ANTES: $1,669 (incorrecto)

3. CONFIG:
   - TC Compra: ₡494.00 (editable, amarillo)
   - TC Venta: ₡508.00 (editable, amarillo)
   - Historial inicia 12/Nov con TCs correctos

EFECTIVO NETO RECALCULADO:
Con TC correcto (494):
- Bancos: $3,505.92 USD equivalente
- Tarjetas: $16,617.17
- NETO: -$13,111.25 (CRISIS)

FUENTE TC:
Usuario confirmó valores oficiales 12/Nov/2025
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -496,7 +496,7 @@
       <text>
         <t>💡 TIPO DE CAMBIO COMPRA
 Cuántos colones TE DAN por $1 USD
-Ejemplo: Si banco te da ₡517.50 por $1
+Ejemplo: Si banco te da ₡494.00 por $1
 ⚠️ Actualizar 1 vez/semana</t>
       </text>
     </comment>
@@ -504,7 +504,7 @@
       <text>
         <t>💡 TIPO DE CAMBIO VENTA
 Cuántos colones PAGAS por $1 USD
-Ejemplo: Si banco cobra ₡525.00 por $1
+Ejemplo: Si banco cobra ₡508.00 por $1
 ⚠️ Actualizar 1 vez/semana</t>
       </text>
     </comment>
@@ -1453,7 +1453,7 @@
         </is>
       </c>
       <c r="E14" s="13">
-        <f>SUMIF(D5:D13,"USD",E5:E13)+SUMIF(D5:D13,"CRC",E5:E13)/517.5</f>
+        <f>SUMIF(D5:D13,"USD",E5:E13)+SUMIF(D5:D13,"CRC",E5:E13)/494.0</f>
         <v/>
       </c>
       <c r="F14" s="13">
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="16">
-        <f>C18+(D18/517.5)</f>
+        <f>C18+(D18/494)</f>
         <v/>
       </c>
       <c r="F18" s="16" t="n">
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="16">
-        <f>C19+(D19/517.5)</f>
+        <f>C19+(D19/494)</f>
         <v/>
       </c>
       <c r="F19" s="16" t="n">
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="16">
-        <f>C20+(D20/517.5)</f>
+        <f>C20+(D20/494)</f>
         <v/>
       </c>
       <c r="F20" s="16" t="n">
@@ -1652,7 +1652,7 @@
         <v>863830</v>
       </c>
       <c r="E21" s="16">
-        <f>C21+(D21/517.5)</f>
+        <f>C21+(D21/494)</f>
         <v/>
       </c>
       <c r="F21" s="16" t="n">
@@ -1689,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="16">
-        <f>C22+(D22/517.5)</f>
+        <f>C22+(D22/494)</f>
         <v/>
       </c>
       <c r="F22" s="16" t="n">
@@ -1774,14 +1774,14 @@
     <row r="30">
       <c r="A30" s="18" t="inlineStr">
         <is>
-          <t>• Tipo de cambio usado: ₡517.5 por $1 USD</t>
+          <t>• Tipo de cambio usado para conversión: TC Compra ₡494.00 por $1 USD (12/Nov/2025)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="24" t="inlineStr">
         <is>
-          <t>• EFECTIVO NETO REAL (12/Nov): $3,444.54 en bancos - $16,536 en tarjetas = -$13,091.46 (CRISIS)</t>
+          <t>• EFECTIVO NETO REAL: Bancos - Tarjetas (ver cálculo arriba)</t>
         </is>
       </c>
     </row>
@@ -3419,7 +3419,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13/11/2025 00:24</t>
+          <t>13/11/2025 00:28</t>
         </is>
       </c>
     </row>
@@ -3495,11 +3495,11 @@
         </is>
       </c>
       <c r="B12" s="9" t="n">
-        <v>517.5</v>
+        <v>494</v>
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:24</t>
+          <t>13/11/2025 00:28</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3515,11 +3515,11 @@
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:24</t>
+          <t>13/11/2025 00:28</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -3574,10 +3574,10 @@
         </is>
       </c>
       <c r="B17" s="34" t="n">
-        <v>517.5</v>
+        <v>494</v>
       </c>
       <c r="C17" s="34" t="n">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="D17" s="35">
         <f>(B17+C17)/2</f>

</xml_diff>

<commit_message>
FIX: Excel v3.0 con datos REALES del cuestionario
✅ CORRECCIONES APLICADAS:
- 22 clientes REALES (no ejemplos inventados)
- 9 cuentas bancarias completas (5 BNCR + 4 Promerica)
- 5 tarjetas de crédito integradas en EFECTIVO
- TC Real 12/Nov: Compra ₡494.00, Venta ₡508.00
- Propietario: Alvaro Velasco - AVN (AlvaroVelascoNet)
- Sistema bi-moneda con historial TC en CONFIG
- CxC pre-cargados (,923.19 total) para FASE 2

📊 ESTRUCTURA EFECTIVO:
- Sección 1: Cuentas Bancarias (ACTIVOS) = ,506 USD equiv
- Sección 2: Tarjetas Crédito (PASIVOS) = 6,617 USD equiv
- Sección 3: Efectivo Neto = -3,111 USD

🎯 FASE 1 MVP: 100% COMPLETA
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -3419,7 +3419,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13/11/2025 00:28</t>
+          <t>13/11/2025 00:36</t>
         </is>
       </c>
     </row>
@@ -3499,7 +3499,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:28</t>
+          <t>13/11/2025 00:36</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:28</t>
+          <t>13/11/2025 00:36</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">

</xml_diff>

<commit_message>
FIX: Excel v3.0 con TC correcto y GASTO PERSONAL
✅ CORRECCIONES APLICADAS:
- Columna J (TC): ₡540 → ₡508 (TC Venta)
- Nuevo tipo: GASTO PERSONAL (gastos no deducibles)
- Dropdown actualizado con 9 tipos de transacción
- Manual inline actualizado

📊 VALIDACIÓN:
- TC 508 correcto para transacciones normales
- GASTO PERSONAL ahora disponible en dropdown
- 5 columnas de alias en ENTIDADES_ALIAS (expandible)
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -332,6 +332,7 @@
 Opciones:
 • INGRESO - Dinero que entra
 • GASTO OPERATIVO - Gastos del negocio
+• GASTO PERSONAL - Gastos personales/no deducibles
 • GASTO FINANCIERO - Intereses, comisiones
 • COMPRA PARA REVENTA - Inventario
 • TRANSFERENCIA - Movimiento entre cuentas
@@ -407,9 +408,10 @@
     <comment ref="J2" authorId="0" shapeId="0">
       <text>
         <t>💡 TIPO DE CAMBIO
-Ingresa el tipo de cambio del día.
-Si dejas vacío, se usará 540 por defecto.
-Formato: 540 (sin comas)</t>
+Ingresa el TC del día de la transacción.
+Por defecto: ₡508 (TC Venta 12/Nov/2025)
+Actualiza en CONFIG si cambia.
+Formato: 508 (sin comas)</t>
       </text>
     </comment>
     <comment ref="K2" authorId="0" shapeId="0">
@@ -945,7 +947,7 @@
       <c r="H2" s="4" t="n"/>
       <c r="I2" s="4" t="n"/>
       <c r="J2" s="4" t="n">
-        <v>540</v>
+        <v>508</v>
       </c>
       <c r="K2" s="3" t="n"/>
       <c r="L2" s="3" t="n"/>
@@ -977,7 +979,7 @@
   </sheetData>
   <dataValidations count="6">
     <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Tipo inválido" error="Selecciona un tipo válido de la lista" type="list">
-      <formula1>"INGRESO,GASTO OPERATIVO,GASTO FINANCIERO,COMPRA PARA REVENTA,TRANSFERENCIA,PAGO TARJETA,PAGO PRESTAMO,AJUSTE"</formula1>
+      <formula1>"INGRESO,GASTO OPERATIVO,GASTO PERSONAL,GASTO FINANCIERO,COMPRA PARA REVENTA,TRANSFERENCIA,PAGO TARJETA,PAGO PRESTAMO,AJUSTE"</formula1>
     </dataValidation>
     <dataValidation sqref="C2:C1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Categoría inválida" error="Selecciona una categoría válida de la lista" type="list">
       <formula1>"Ventas - Servicios Técnicos,Ventas - Hardware,Ventas - Software,Compras - Inventario,Salarios,Seguridad Social (CCSS),Alquiler,Servicios Públicos,Internet/Teléfono,Combustible,Mantenimiento,Papelería,Intereses - Tarjetas,Intereses - Préstamos,Intereses - Hacienda,IVA Cobrado,IVA Pagado,Transferencia entre cuentas,Otros"</formula1>
@@ -3419,7 +3421,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>13/11/2025 00:36</t>
+          <t>13/11/2025 00:54</t>
         </is>
       </c>
     </row>
@@ -3499,7 +3501,7 @@
       </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:36</t>
+          <t>13/11/2025 00:54</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -3519,7 +3521,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>13/11/2025 00:36</t>
+          <t>13/11/2025 00:54</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">

</xml_diff>

<commit_message>
UPDATE: CxP con Nissan y Hacienda corregidos - Nissan: /mes financiamiento - Hacienda: Prioridad BAJA (arreglo pago) - Total CxP: ,509.33 - Neto: -,841.13
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -13,6 +13,8 @@
     <sheet name="CONFIG" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="CxC" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="CxP" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="CxC1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="CxP1" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -13641,4 +13643,1294 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" style="36" min="1" max="1"/>
+    <col width="12" customWidth="1" style="36" min="2" max="2"/>
+    <col width="12" customWidth="1" style="36" min="3" max="3"/>
+    <col width="12" customWidth="1" style="36" min="4" max="4"/>
+    <col width="10" customWidth="1" style="36" min="5" max="5"/>
+    <col width="12" customWidth="1" style="36" min="6" max="6"/>
+    <col width="12" customWidth="1" style="36" min="7" max="7"/>
+    <col width="12" customWidth="1" style="36" min="8" max="8"/>
+    <col width="12" customWidth="1" style="36" min="9" max="9"/>
+    <col width="30" customWidth="1" style="36" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="58" t="inlineStr">
+        <is>
+          <t>CUENTAS POR COBRAR (CxC)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="59" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="B2" s="59" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="C2" s="59" t="inlineStr">
+        <is>
+          <t>Fecha Emisión</t>
+        </is>
+      </c>
+      <c r="D2" s="59" t="inlineStr">
+        <is>
+          <t>Fecha Vencimiento</t>
+        </is>
+      </c>
+      <c r="E2" s="59" t="inlineStr">
+        <is>
+          <t>Días Crédito</t>
+        </is>
+      </c>
+      <c r="F2" s="59" t="inlineStr">
+        <is>
+          <t>Monto USD</t>
+        </is>
+      </c>
+      <c r="G2" s="59" t="inlineStr">
+        <is>
+          <t>Saldo USD</t>
+        </is>
+      </c>
+      <c r="H2" s="59" t="inlineStr">
+        <is>
+          <t>Días Vencido</t>
+        </is>
+      </c>
+      <c r="I2" s="59" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="J2" s="59" t="inlineStr">
+        <is>
+          <t>Notas</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Grupo Acción Comercial S.A.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>AR-002</t>
+        </is>
+      </c>
+      <c r="C3" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D3" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E3" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" s="51" t="n">
+        <v>1689.04</v>
+      </c>
+      <c r="G3" s="51" t="n">
+        <v>1689.04</v>
+      </c>
+      <c r="H3" s="60">
+        <f>IF(D3&lt;TODAY(), TODAY()-D3, 0)</f>
+        <v/>
+      </c>
+      <c r="I3">
+        <f>IF(H3=0, "AL DÍA", IF(H3&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>VWR International Ltda</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AR-001</t>
+        </is>
+      </c>
+      <c r="C4" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D4" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E4" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="51" t="n">
+        <v>3567.08</v>
+      </c>
+      <c r="G4" s="51" t="n">
+        <v>3567.08</v>
+      </c>
+      <c r="H4" s="60">
+        <f>IF(D4&lt;TODAY(), TODAY()-D4, 0)</f>
+        <v/>
+      </c>
+      <c r="I4">
+        <f>IF(H4=0, "AL DÍA", IF(H4&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3-102-887892 SRL</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AR-004</t>
+        </is>
+      </c>
+      <c r="C5" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D5" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E5" t="n">
+        <v>30</v>
+      </c>
+      <c r="F5" s="51" t="n">
+        <v>691.5599999999999</v>
+      </c>
+      <c r="G5" s="51" t="n">
+        <v>691.5599999999999</v>
+      </c>
+      <c r="H5" s="60">
+        <f>IF(D5&lt;TODAY(), TODAY()-D5, 0)</f>
+        <v/>
+      </c>
+      <c r="I5">
+        <f>IF(H5=0, "AL DÍA", IF(H5&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Centro Integral Oncología CIO SRL</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>AR-006</t>
+        </is>
+      </c>
+      <c r="C6" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D6" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E6" t="n">
+        <v>30</v>
+      </c>
+      <c r="F6" s="51" t="n">
+        <v>687.05</v>
+      </c>
+      <c r="G6" s="51" t="n">
+        <v>687.05</v>
+      </c>
+      <c r="H6" s="60">
+        <f>IF(D6&lt;TODAY(), TODAY()-D6, 0)</f>
+        <v/>
+      </c>
+      <c r="I6">
+        <f>IF(H6=0, "AL DÍA", IF(H6&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ortodoncia de la Cruz</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AR-007</t>
+        </is>
+      </c>
+      <c r="C7" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D7" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E7" t="n">
+        <v>30</v>
+      </c>
+      <c r="F7" s="51" t="n">
+        <v>494.5</v>
+      </c>
+      <c r="G7" s="51" t="n">
+        <v>494.5</v>
+      </c>
+      <c r="H7" s="60">
+        <f>IF(D7&lt;TODAY(), TODAY()-D7, 0)</f>
+        <v/>
+      </c>
+      <c r="I7">
+        <f>IF(H7=0, "AL DÍA", IF(H7&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Global Automotriz GACR S.A.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AR-008</t>
+        </is>
+      </c>
+      <c r="C8" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D8" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E8" t="n">
+        <v>30</v>
+      </c>
+      <c r="F8" s="51" t="n">
+        <v>439.61</v>
+      </c>
+      <c r="G8" s="51" t="n">
+        <v>439.61</v>
+      </c>
+      <c r="H8" s="60">
+        <f>IF(D8&lt;TODAY(), TODAY()-D8, 0)</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>IF(H8=0, "AL DÍA", IF(H8&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Solusa Consolidators</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>AR-009</t>
+        </is>
+      </c>
+      <c r="C9" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D9" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E9" t="n">
+        <v>30</v>
+      </c>
+      <c r="F9" s="51" t="n">
+        <v>378.35</v>
+      </c>
+      <c r="G9" s="51" t="n">
+        <v>378.35</v>
+      </c>
+      <c r="H9" s="60">
+        <f>IF(D9&lt;TODAY(), TODAY()-D9, 0)</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>IF(H9=0, "AL DÍA", IF(H9&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Cemso</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AR-010</t>
+        </is>
+      </c>
+      <c r="C10" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D10" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F10" s="51" t="n">
+        <v>333.92</v>
+      </c>
+      <c r="G10" s="51" t="n">
+        <v>333.92</v>
+      </c>
+      <c r="H10" s="60">
+        <f>IF(D10&lt;TODAY(), TODAY()-D10, 0)</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>IF(H10=0, "AL DÍA", IF(H10&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Rodriguez Rojas Carlos Humberto</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AR-012</t>
+        </is>
+      </c>
+      <c r="C11" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D11" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" s="51" t="n">
+        <v>282.5</v>
+      </c>
+      <c r="G11" s="51" t="n">
+        <v>282.5</v>
+      </c>
+      <c r="H11" s="60">
+        <f>IF(D11&lt;TODAY(), TODAY()-D11, 0)</f>
+        <v/>
+      </c>
+      <c r="I11">
+        <f>IF(H11=0, "AL DÍA", IF(H11&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Supply Net C.R.W.H S.A.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>AR-013</t>
+        </is>
+      </c>
+      <c r="C12" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D12" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F12" s="51" t="n">
+        <v>276.85</v>
+      </c>
+      <c r="G12" s="51" t="n">
+        <v>276.85</v>
+      </c>
+      <c r="H12" s="60">
+        <f>IF(D12&lt;TODAY(), TODAY()-D12, 0)</f>
+        <v/>
+      </c>
+      <c r="I12">
+        <f>IF(H12=0, "AL DÍA", IF(H12&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Operation Managment Tierra Magnifica</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AR-014</t>
+        </is>
+      </c>
+      <c r="C13" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D13" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E13" t="n">
+        <v>30</v>
+      </c>
+      <c r="F13" s="51" t="n">
+        <v>209.06</v>
+      </c>
+      <c r="G13" s="51" t="n">
+        <v>209.06</v>
+      </c>
+      <c r="H13" s="60">
+        <f>IF(D13&lt;TODAY(), TODAY()-D13, 0)</f>
+        <v/>
+      </c>
+      <c r="I13">
+        <f>IF(H13=0, "AL DÍA", IF(H13&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Sevilla Navarro Edgar</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AR-016</t>
+        </is>
+      </c>
+      <c r="C14" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D14" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E14" t="n">
+        <v>30</v>
+      </c>
+      <c r="F14" s="51" t="n">
+        <v>169.5</v>
+      </c>
+      <c r="G14" s="51" t="n">
+        <v>169.5</v>
+      </c>
+      <c r="H14" s="60">
+        <f>IF(D14&lt;TODAY(), TODAY()-D14, 0)</f>
+        <v/>
+      </c>
+      <c r="I14">
+        <f>IF(H14=0, "AL DÍA", IF(H14&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Gomez Ajoy Edgar Luis</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AR-017</t>
+        </is>
+      </c>
+      <c r="C15" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D15" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E15" t="n">
+        <v>30</v>
+      </c>
+      <c r="F15" s="51" t="n">
+        <v>113</v>
+      </c>
+      <c r="G15" s="51" t="n">
+        <v>113</v>
+      </c>
+      <c r="H15" s="60">
+        <f>IF(D15&lt;TODAY(), TODAY()-D15, 0)</f>
+        <v/>
+      </c>
+      <c r="I15">
+        <f>IF(H15=0, "AL DÍA", IF(H15&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Melendez Morales Monica</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AR-018</t>
+        </is>
+      </c>
+      <c r="C16" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D16" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E16" t="n">
+        <v>30</v>
+      </c>
+      <c r="F16" s="51" t="n">
+        <v>113</v>
+      </c>
+      <c r="G16" s="51" t="n">
+        <v>113</v>
+      </c>
+      <c r="H16" s="60">
+        <f>IF(D16&lt;TODAY(), TODAY()-D16, 0)</f>
+        <v/>
+      </c>
+      <c r="I16">
+        <f>IF(H16=0, "AL DÍA", IF(H16&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Bandogo Soluciones Tecnológicas S.A.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AR-019</t>
+        </is>
+      </c>
+      <c r="C17" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D17" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E17" t="n">
+        <v>30</v>
+      </c>
+      <c r="F17" s="51" t="n">
+        <v>67.8</v>
+      </c>
+      <c r="G17" s="51" t="n">
+        <v>67.8</v>
+      </c>
+      <c r="H17" s="60">
+        <f>IF(D17&lt;TODAY(), TODAY()-D17, 0)</f>
+        <v/>
+      </c>
+      <c r="I17">
+        <f>IF(H17=0, "AL DÍA", IF(H17&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>CPF Servicios Radiológicos S.A.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>AR-020</t>
+        </is>
+      </c>
+      <c r="C18" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D18" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E18" t="n">
+        <v>30</v>
+      </c>
+      <c r="F18" s="51" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="G18" s="51" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="H18" s="60">
+        <f>IF(D18&lt;TODAY(), TODAY()-D18, 0)</f>
+        <v/>
+      </c>
+      <c r="I18">
+        <f>IF(H18=0, "AL DÍA", IF(H18&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ortodec S.A.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>AR-021</t>
+        </is>
+      </c>
+      <c r="C19" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D19" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E19" t="n">
+        <v>30</v>
+      </c>
+      <c r="F19" s="51" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="G19" s="51" t="n">
+        <v>56.5</v>
+      </c>
+      <c r="H19" s="60">
+        <f>IF(D19&lt;TODAY(), TODAY()-D19, 0)</f>
+        <v/>
+      </c>
+      <c r="I19">
+        <f>IF(H19=0, "AL DÍA", IF(H19&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Perez Morales Francisco</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AR-022</t>
+        </is>
+      </c>
+      <c r="C20" s="49" t="n">
+        <v>45962</v>
+      </c>
+      <c r="D20" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="E20" t="n">
+        <v>30</v>
+      </c>
+      <c r="F20" s="51" t="n">
+        <v>42.38</v>
+      </c>
+      <c r="G20" s="51" t="n">
+        <v>42.38</v>
+      </c>
+      <c r="H20" s="60">
+        <f>IF(D20&lt;TODAY(), TODAY()-D20, 0)</f>
+        <v/>
+      </c>
+      <c r="I20">
+        <f>IF(H20=0, "AL DÍA", IF(H20&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="61" t="inlineStr">
+        <is>
+          <t>TOTAL CxC</t>
+        </is>
+      </c>
+      <c r="F21" s="62">
+        <f>SUM(F3:F20)</f>
+        <v/>
+      </c>
+      <c r="G21" s="62">
+        <f>SUM(G3:G20)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" style="36" min="1" max="1"/>
+    <col width="15" customWidth="1" style="36" min="2" max="2"/>
+    <col width="12" customWidth="1" style="36" min="3" max="3"/>
+    <col width="12" customWidth="1" style="36" min="4" max="4"/>
+    <col width="12" customWidth="1" style="36" min="5" max="5"/>
+    <col width="12" customWidth="1" style="36" min="6" max="6"/>
+    <col width="12" customWidth="1" style="36" min="7" max="7"/>
+    <col width="12" customWidth="1" style="36" min="8" max="8"/>
+    <col width="12" customWidth="1" style="36" min="9" max="9"/>
+    <col width="30" customWidth="1" style="36" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="63" t="inlineStr">
+        <is>
+          <t>CUENTAS POR PAGAR (CxP)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="59" t="inlineStr">
+        <is>
+          <t>Proveedor</t>
+        </is>
+      </c>
+      <c r="B2" s="59" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="C2" s="59" t="inlineStr">
+        <is>
+          <t>Fecha Emisión</t>
+        </is>
+      </c>
+      <c r="D2" s="59" t="inlineStr">
+        <is>
+          <t>Fecha Vencimiento</t>
+        </is>
+      </c>
+      <c r="E2" s="59" t="inlineStr">
+        <is>
+          <t>Monto USD</t>
+        </is>
+      </c>
+      <c r="F2" s="59" t="inlineStr">
+        <is>
+          <t>Saldo USD</t>
+        </is>
+      </c>
+      <c r="G2" s="59" t="inlineStr">
+        <is>
+          <t>Días Vencido</t>
+        </is>
+      </c>
+      <c r="H2" s="59" t="inlineStr">
+        <is>
+          <t>Prioridad</t>
+        </is>
+      </c>
+      <c r="I2" s="59" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="J2" s="59" t="inlineStr">
+        <is>
+          <t>Notas</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intcomex Costa Rica</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2518439</t>
+        </is>
+      </c>
+      <c r="C3" s="49" t="n">
+        <v>45964</v>
+      </c>
+      <c r="D3" s="49" t="n">
+        <v>45994</v>
+      </c>
+      <c r="E3" s="51" t="n">
+        <v>2317.09</v>
+      </c>
+      <c r="F3" s="51" t="n">
+        <v>2317.09</v>
+      </c>
+      <c r="G3" s="60">
+        <f>IF(D3&lt;TODAY(), TODAY()-D3, 0)</f>
+        <v/>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="I3">
+        <f>IF(G3=0, "AL DÍA", IF(G3&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Intcomex Costa Rica</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2518765</t>
+        </is>
+      </c>
+      <c r="C4" s="49" t="n">
+        <v>45965</v>
+      </c>
+      <c r="D4" s="49" t="n">
+        <v>45995</v>
+      </c>
+      <c r="E4" s="51" t="n">
+        <v>679.12</v>
+      </c>
+      <c r="F4" s="51" t="n">
+        <v>679.12</v>
+      </c>
+      <c r="G4" s="60">
+        <f>IF(D4&lt;TODAY(), TODAY()-D4, 0)</f>
+        <v/>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="I4">
+        <f>IF(G4=0, "AL DÍA", IF(G4&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Intcomex Costa Rica</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2520652</t>
+        </is>
+      </c>
+      <c r="C5" s="49" t="n">
+        <v>45971</v>
+      </c>
+      <c r="D5" s="49" t="n">
+        <v>46001</v>
+      </c>
+      <c r="E5" s="51" t="n">
+        <v>565.34</v>
+      </c>
+      <c r="F5" s="51" t="n">
+        <v>565.34</v>
+      </c>
+      <c r="G5" s="60">
+        <f>IF(D5&lt;TODAY(), TODAY()-D5, 0)</f>
+        <v/>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="I5">
+        <f>IF(G5=0, "AL DÍA", IF(G5&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alquiler Oficina</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Mensual</t>
+        </is>
+      </c>
+      <c r="C6" s="49" t="n">
+        <v>45976</v>
+      </c>
+      <c r="D6" s="49" t="n">
+        <v>46006</v>
+      </c>
+      <c r="E6" s="51" t="n">
+        <v>775</v>
+      </c>
+      <c r="F6" s="51" t="n">
+        <v>775</v>
+      </c>
+      <c r="G6" s="60">
+        <f>IF(D6&lt;TODAY(), TODAY()-D6, 0)</f>
+        <v/>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>CRÍTICA</t>
+        </is>
+      </c>
+      <c r="I6">
+        <f>IF(G6=0, "AL DÍA", IF(G6&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Nissan - Financiamiento</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Cuota mensual</t>
+        </is>
+      </c>
+      <c r="C7" s="49" t="n">
+        <v>45976</v>
+      </c>
+      <c r="D7" s="49" t="n">
+        <v>46006</v>
+      </c>
+      <c r="E7" s="51" t="n">
+        <v>800</v>
+      </c>
+      <c r="F7" s="51" t="n">
+        <v>800</v>
+      </c>
+      <c r="G7" s="60">
+        <f>IF(D7&lt;TODAY(), TODAY()-D7, 0)</f>
+        <v/>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="I7">
+        <f>IF(G7=0, "AL DÍA", IF(G7&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hacienda - IVA/Renta</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Arreglo de pago</t>
+        </is>
+      </c>
+      <c r="C8" s="49" t="n">
+        <v>45992</v>
+      </c>
+      <c r="D8" s="49" t="n">
+        <v>46022</v>
+      </c>
+      <c r="E8" s="51" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="51" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G8" s="60">
+        <f>IF(D8&lt;TODAY(), TODAY()-D8, 0)</f>
+        <v/>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>BAJA</t>
+        </is>
+      </c>
+      <c r="I8">
+        <f>IF(G8=0, "AL DÍA", IF(G8&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sea Global Logistics (SGL)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Importación 1</t>
+        </is>
+      </c>
+      <c r="C9" s="49" t="n">
+        <v>45944</v>
+      </c>
+      <c r="D9" s="49" t="n">
+        <v>45974</v>
+      </c>
+      <c r="E9" s="51" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="F9" s="51" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="G9" s="60">
+        <f>IF(D9&lt;TODAY(), TODAY()-D9, 0)</f>
+        <v/>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="I9">
+        <f>IF(G9=0, "AL DÍA", IF(G9&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Sea Global Logistics (SGL)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Importación 2</t>
+        </is>
+      </c>
+      <c r="C10" s="49" t="n">
+        <v>45944</v>
+      </c>
+      <c r="D10" s="49" t="n">
+        <v>45974</v>
+      </c>
+      <c r="E10" s="51" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="F10" s="51" t="n">
+        <v>14.69</v>
+      </c>
+      <c r="G10" s="60">
+        <f>IF(D10&lt;TODAY(), TODAY()-D10, 0)</f>
+        <v/>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="I10">
+        <f>IF(G10=0, "AL DÍA", IF(G10&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Corporacion Geoalerta TTI, S.A.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Seguridad Sept</t>
+        </is>
+      </c>
+      <c r="C11" s="49" t="n">
+        <v>45944</v>
+      </c>
+      <c r="D11" s="49" t="n">
+        <v>45974</v>
+      </c>
+      <c r="E11" s="51" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="F11" s="51" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="G11" s="60">
+        <f>IF(D11&lt;TODAY(), TODAY()-D11, 0)</f>
+        <v/>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="I11">
+        <f>IF(G11=0, "AL DÍA", IF(G11&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Computadores Economicos, S.A.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LCD/Bateria/Pantalla</t>
+        </is>
+      </c>
+      <c r="C12" s="49" t="n">
+        <v>45954</v>
+      </c>
+      <c r="D12" s="49" t="n">
+        <v>45984</v>
+      </c>
+      <c r="E12" s="51" t="n">
+        <v>284.9</v>
+      </c>
+      <c r="F12" s="51" t="n">
+        <v>284.9</v>
+      </c>
+      <c r="G12" s="60">
+        <f>IF(D12&lt;TODAY(), TODAY()-D12, 0)</f>
+        <v/>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="I12">
+        <f>IF(G12=0, "AL DÍA", IF(G12&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Eurocomp de Costa Rica, S.A.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Teclado/Mouse</t>
+        </is>
+      </c>
+      <c r="C13" s="49" t="n">
+        <v>45950</v>
+      </c>
+      <c r="D13" s="49" t="n">
+        <v>45980</v>
+      </c>
+      <c r="E13" s="51" t="n">
+        <v>16.92</v>
+      </c>
+      <c r="F13" s="51" t="n">
+        <v>16.92</v>
+      </c>
+      <c r="G13" s="60">
+        <f>IF(D13&lt;TODAY(), TODAY()-D13, 0)</f>
+        <v/>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="I13">
+        <f>IF(G13=0, "AL DÍA", IF(G13&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Eurocomp de Costa Rica, S.A.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PC/Laptop/UPS/Monitor</t>
+        </is>
+      </c>
+      <c r="C14" s="49" t="n">
+        <v>45947</v>
+      </c>
+      <c r="D14" s="49" t="n">
+        <v>45977</v>
+      </c>
+      <c r="E14" s="51" t="n">
+        <v>2007.68</v>
+      </c>
+      <c r="F14" s="51" t="n">
+        <v>2007.68</v>
+      </c>
+      <c r="G14" s="60">
+        <f>IF(D14&lt;TODAY(), TODAY()-D14, 0)</f>
+        <v/>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>ALTA</t>
+        </is>
+      </c>
+      <c r="I14">
+        <f>IF(G14=0, "AL DÍA", IF(G14&lt;=15, "POR VENCER", "VENCIDA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="64" t="inlineStr">
+        <is>
+          <t>TOTAL CxP</t>
+        </is>
+      </c>
+      <c r="E15" s="62">
+        <f>SUM(E3:E14)</f>
+        <v/>
+      </c>
+      <c r="F15" s="62">
+        <f>SUM(F3:F14)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ADD: FASE 3 IVA_CONTROL + limpieza duplicados
- Script limpiar_duplicados_cxc_cxp.py: Elimina CxC/CxP antiguos
- Script agregar_iva_control_fase3.py: Control IVA Costa Rica
- Hoja IVA_CONTROL con 3 secciones:
  * Ventas: IVA 13% cobrado, retención 2%, zona franca
  * Compras: IVA acreditable, gastos deducibles
  * Resumen D-104: IVA neto a pagar
- Fórmulas automáticas para cálculos IVA
- Vencimiento: 26/Nov/2025
- Excel v3.0: 8 hojas completas
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TRANSACCIONES" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="EFECTIVO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="DASHBOARD" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="ENTIDADES_ALIAS" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="CONFIG" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="CxC" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="CxP" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="CxC1" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="CxP1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TRANSACCIONES" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EFECTIVO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DASHBOARD" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ENTIDADES_ALIAS" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONFIG" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="IVA_CONTROL" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CxC" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CxP" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -23,7 +22,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="\₡#,##0.00"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\₡#,##0"/>
@@ -33,9 +32,8 @@
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="171" formatCode="₡#,##0.00"/>
     <numFmt numFmtId="172" formatCode="$#,##0.00"/>
-    <numFmt numFmtId="173" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,8 +155,22 @@
       <b val="1"/>
       <color rgb="00FF0000"/>
     </font>
+    <font>
+      <i val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FF0000"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill/>
     </fill>
@@ -207,6 +219,42 @@
         <bgColor rgb="001F4E78"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+        <bgColor rgb="00E7E6E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ADD8E6"/>
+        <bgColor rgb="00ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE4D6"/>
+        <bgColor rgb="00FCE4D6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -241,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -355,6 +403,18 @@
     <xf numFmtId="172" fontId="18" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="10" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="18" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="18" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="11" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="23" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12398,7 +12458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12406,1246 +12466,952 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" style="36" min="1" max="1"/>
+    <col width="10" customWidth="1" style="36" min="1" max="1"/>
     <col width="12" customWidth="1" style="36" min="2" max="2"/>
-    <col width="12" customWidth="1" style="36" min="3" max="3"/>
-    <col width="12" customWidth="1" style="36" min="4" max="4"/>
-    <col width="10" customWidth="1" style="36" min="5" max="5"/>
-    <col width="12" customWidth="1" style="36" min="6" max="6"/>
-    <col width="12" customWidth="1" style="36" min="7" max="7"/>
+    <col width="30" customWidth="1" style="36" min="3" max="3"/>
+    <col width="14" customWidth="1" style="36" min="4" max="4"/>
+    <col width="14" customWidth="1" style="36" min="5" max="5"/>
+    <col width="14" customWidth="1" style="36" min="6" max="6"/>
+    <col width="10" customWidth="1" style="36" min="7" max="7"/>
     <col width="12" customWidth="1" style="36" min="8" max="8"/>
-    <col width="12" customWidth="1" style="36" min="9" max="9"/>
-    <col width="30" customWidth="1" style="36" min="10" max="10"/>
+    <col width="14" customWidth="1" style="36" min="9" max="9"/>
+    <col width="10" customWidth="1" style="36" min="10" max="10"/>
+    <col width="10" customWidth="1" style="36" min="11" max="11"/>
+    <col width="20" customWidth="1" style="36" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="58" t="inlineStr">
         <is>
-          <t>CUENTAS POR COBRAR (CxC)</t>
+          <t>CONTROL DE IVA - COSTA RICA</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="59" t="inlineStr">
+      <c r="A2" s="65" t="inlineStr">
+        <is>
+          <t>Período: NOVIEMBRE 2025 | Vencimiento D-104: 26/Nov/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="66" t="inlineStr">
+        <is>
+          <t>VENTAS - IVA COBRADO (13%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="59" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B5" s="59" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="C5" s="59" t="inlineStr">
         <is>
           <t>Cliente</t>
         </is>
       </c>
-      <c r="B2" s="59" t="inlineStr">
-        <is>
-          <t>Factura</t>
-        </is>
-      </c>
-      <c r="C2" s="59" t="inlineStr">
-        <is>
-          <t>Fecha Emisión</t>
-        </is>
-      </c>
-      <c r="D2" s="59" t="inlineStr">
-        <is>
-          <t>Fecha Vencimiento</t>
-        </is>
-      </c>
-      <c r="E2" s="59" t="inlineStr">
-        <is>
-          <t>Días Crédito</t>
-        </is>
-      </c>
-      <c r="F2" s="59" t="inlineStr">
-        <is>
-          <t>Monto USD</t>
-        </is>
-      </c>
-      <c r="G2" s="59" t="inlineStr">
-        <is>
-          <t>Saldo USD</t>
-        </is>
-      </c>
-      <c r="H2" s="59" t="inlineStr">
-        <is>
-          <t>Días Vencido</t>
-        </is>
-      </c>
-      <c r="I2" s="59" t="inlineStr">
+      <c r="D5" s="59" t="inlineStr">
+        <is>
+          <t>Base Gravable USD</t>
+        </is>
+      </c>
+      <c r="E5" s="59" t="inlineStr">
+        <is>
+          <t>IVA 13% USD</t>
+        </is>
+      </c>
+      <c r="F5" s="59" t="inlineStr">
+        <is>
+          <t>Total USD</t>
+        </is>
+      </c>
+      <c r="G5" s="59" t="inlineStr">
+        <is>
+          <t>Zona Franca</t>
+        </is>
+      </c>
+      <c r="H5" s="59" t="inlineStr">
+        <is>
+          <t>Retención 2%</t>
+        </is>
+      </c>
+      <c r="I5" s="59" t="inlineStr">
+        <is>
+          <t>Neto Cobrado</t>
+        </is>
+      </c>
+      <c r="J5" s="59" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="J2" s="59" t="inlineStr">
+      <c r="K5" s="59" t="inlineStr">
+        <is>
+          <t>Ref Trans</t>
+        </is>
+      </c>
+      <c r="L5" s="59" t="inlineStr">
         <is>
           <t>Notas</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Grupo Acción Comercial S.A.</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>AR-002</t>
-        </is>
-      </c>
-      <c r="C3" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D3" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E3" t="n">
-        <v>30</v>
-      </c>
-      <c r="F3" s="51" t="n">
-        <v>1689.04</v>
-      </c>
-      <c r="G3" s="51" t="n">
-        <v>1689.04</v>
-      </c>
-      <c r="H3" s="60">
-        <f>IF(D3&lt;TODAY(), TODAY()-D3, 0)</f>
-        <v/>
-      </c>
-      <c r="I3">
-        <f>IF(H3=0, "AL DÍA", IF(H3&lt;=30, "VENCIDA", "CRÍTICA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>VWR International Ltda</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>AR-001</t>
-        </is>
-      </c>
-      <c r="C4" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D4" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E4" t="n">
-        <v>30</v>
-      </c>
-      <c r="F4" s="51" t="n">
-        <v>3567.08</v>
-      </c>
-      <c r="G4" s="51" t="n">
-        <v>3567.08</v>
-      </c>
-      <c r="H4" s="60">
-        <f>IF(D4&lt;TODAY(), TODAY()-D4, 0)</f>
-        <v/>
-      </c>
-      <c r="I4">
-        <f>IF(H4=0, "AL DÍA", IF(H4&lt;=30, "VENCIDA", "CRÍTICA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>3-102-887892 SRL</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>AR-004</t>
-        </is>
-      </c>
-      <c r="C5" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D5" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E5" t="n">
-        <v>30</v>
-      </c>
-      <c r="F5" s="51" t="n">
-        <v>691.5599999999999</v>
-      </c>
-      <c r="G5" s="51" t="n">
-        <v>691.5599999999999</v>
-      </c>
-      <c r="H5" s="60">
-        <f>IF(D5&lt;TODAY(), TODAY()-D5, 0)</f>
-        <v/>
-      </c>
-      <c r="I5">
-        <f>IF(H5=0, "AL DÍA", IF(H5&lt;=30, "VENCIDA", "CRÍTICA"))</f>
-        <v/>
-      </c>
-    </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Centro Integral Oncología CIO SRL</t>
+      <c r="A6" s="49" t="inlineStr">
+        <is>
+          <t>01/11/25</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>AR-006</t>
-        </is>
-      </c>
-      <c r="C6" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D6" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E6" t="n">
-        <v>30</v>
-      </c>
-      <c r="F6" s="51" t="n">
-        <v>687.05</v>
-      </c>
-      <c r="G6" s="51" t="n">
-        <v>687.05</v>
-      </c>
-      <c r="H6" s="60">
-        <f>IF(D6&lt;TODAY(), TODAY()-D6, 0)</f>
-        <v/>
-      </c>
-      <c r="I6">
-        <f>IF(H6=0, "AL DÍA", IF(H6&lt;=30, "VENCIDA", "CRÍTICA"))</f>
-        <v/>
+          <t>FAC-001</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Cliente Ejemplo</t>
+        </is>
+      </c>
+      <c r="D6" s="67" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="68">
+        <f>D6*0.13</f>
+        <v/>
+      </c>
+      <c r="F6" s="68">
+        <f>D6+E6</f>
+        <v/>
+      </c>
+      <c r="G6" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="H6" s="68">
+        <f>IF(G6="SI",0,D6*0.02)</f>
+        <v/>
+      </c>
+      <c r="I6" s="68">
+        <f>F6-H6</f>
+        <v/>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ortodoncia de la Cruz</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>AR-007</t>
-        </is>
-      </c>
-      <c r="C7" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D7" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E7" t="n">
-        <v>30</v>
-      </c>
-      <c r="F7" s="51" t="n">
-        <v>494.5</v>
-      </c>
-      <c r="G7" s="51" t="n">
-        <v>494.5</v>
-      </c>
-      <c r="H7" s="60">
-        <f>IF(D7&lt;TODAY(), TODAY()-D7, 0)</f>
-        <v/>
-      </c>
-      <c r="I7">
-        <f>IF(H7=0, "AL DÍA", IF(H7&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A7" s="49" t="n"/>
+      <c r="D7" s="67" t="n"/>
+      <c r="E7" s="68">
+        <f>D7*0.13</f>
+        <v/>
+      </c>
+      <c r="F7" s="68">
+        <f>D7+E7</f>
+        <v/>
+      </c>
+      <c r="G7" s="69" t="n"/>
+      <c r="H7" s="68">
+        <f>IF(G7="SI",0,D7*0.02)</f>
+        <v/>
+      </c>
+      <c r="I7" s="68">
+        <f>F7-H7</f>
         <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Global Automotriz GACR S.A.</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>AR-008</t>
-        </is>
-      </c>
-      <c r="C8" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D8" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E8" t="n">
-        <v>30</v>
-      </c>
-      <c r="F8" s="51" t="n">
-        <v>439.61</v>
-      </c>
-      <c r="G8" s="51" t="n">
-        <v>439.61</v>
-      </c>
-      <c r="H8" s="60">
-        <f>IF(D8&lt;TODAY(), TODAY()-D8, 0)</f>
-        <v/>
-      </c>
-      <c r="I8">
-        <f>IF(H8=0, "AL DÍA", IF(H8&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A8" s="49" t="n"/>
+      <c r="D8" s="67" t="n"/>
+      <c r="E8" s="68">
+        <f>D8*0.13</f>
+        <v/>
+      </c>
+      <c r="F8" s="68">
+        <f>D8+E8</f>
+        <v/>
+      </c>
+      <c r="G8" s="69" t="n"/>
+      <c r="H8" s="68">
+        <f>IF(G8="SI",0,D8*0.02)</f>
+        <v/>
+      </c>
+      <c r="I8" s="68">
+        <f>F8-H8</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Solusa Consolidators</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>AR-009</t>
-        </is>
-      </c>
-      <c r="C9" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D9" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E9" t="n">
-        <v>30</v>
-      </c>
-      <c r="F9" s="51" t="n">
-        <v>378.35</v>
-      </c>
-      <c r="G9" s="51" t="n">
-        <v>378.35</v>
-      </c>
-      <c r="H9" s="60">
-        <f>IF(D9&lt;TODAY(), TODAY()-D9, 0)</f>
-        <v/>
-      </c>
-      <c r="I9">
-        <f>IF(H9=0, "AL DÍA", IF(H9&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A9" s="49" t="n"/>
+      <c r="D9" s="67" t="n"/>
+      <c r="E9" s="68">
+        <f>D9*0.13</f>
+        <v/>
+      </c>
+      <c r="F9" s="68">
+        <f>D9+E9</f>
+        <v/>
+      </c>
+      <c r="G9" s="69" t="n"/>
+      <c r="H9" s="68">
+        <f>IF(G9="SI",0,D9*0.02)</f>
+        <v/>
+      </c>
+      <c r="I9" s="68">
+        <f>F9-H9</f>
         <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Cemso</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>AR-010</t>
-        </is>
-      </c>
-      <c r="C10" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D10" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E10" t="n">
-        <v>30</v>
-      </c>
-      <c r="F10" s="51" t="n">
-        <v>333.92</v>
-      </c>
-      <c r="G10" s="51" t="n">
-        <v>333.92</v>
-      </c>
-      <c r="H10" s="60">
-        <f>IF(D10&lt;TODAY(), TODAY()-D10, 0)</f>
-        <v/>
-      </c>
-      <c r="I10">
-        <f>IF(H10=0, "AL DÍA", IF(H10&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A10" s="49" t="n"/>
+      <c r="D10" s="67" t="n"/>
+      <c r="E10" s="68">
+        <f>D10*0.13</f>
+        <v/>
+      </c>
+      <c r="F10" s="68">
+        <f>D10+E10</f>
+        <v/>
+      </c>
+      <c r="G10" s="69" t="n"/>
+      <c r="H10" s="68">
+        <f>IF(G10="SI",0,D10*0.02)</f>
+        <v/>
+      </c>
+      <c r="I10" s="68">
+        <f>F10-H10</f>
         <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Rodriguez Rojas Carlos Humberto</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>AR-012</t>
-        </is>
-      </c>
-      <c r="C11" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D11" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E11" t="n">
-        <v>30</v>
-      </c>
-      <c r="F11" s="51" t="n">
-        <v>282.5</v>
-      </c>
-      <c r="G11" s="51" t="n">
-        <v>282.5</v>
-      </c>
-      <c r="H11" s="60">
-        <f>IF(D11&lt;TODAY(), TODAY()-D11, 0)</f>
-        <v/>
-      </c>
-      <c r="I11">
-        <f>IF(H11=0, "AL DÍA", IF(H11&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A11" s="49" t="n"/>
+      <c r="D11" s="67" t="n"/>
+      <c r="E11" s="68">
+        <f>D11*0.13</f>
+        <v/>
+      </c>
+      <c r="F11" s="68">
+        <f>D11+E11</f>
+        <v/>
+      </c>
+      <c r="G11" s="69" t="n"/>
+      <c r="H11" s="68">
+        <f>IF(G11="SI",0,D11*0.02)</f>
+        <v/>
+      </c>
+      <c r="I11" s="68">
+        <f>F11-H11</f>
         <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Supply Net C.R.W.H S.A.</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>AR-013</t>
-        </is>
-      </c>
-      <c r="C12" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D12" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E12" t="n">
-        <v>30</v>
-      </c>
-      <c r="F12" s="51" t="n">
-        <v>276.85</v>
-      </c>
-      <c r="G12" s="51" t="n">
-        <v>276.85</v>
-      </c>
-      <c r="H12" s="60">
-        <f>IF(D12&lt;TODAY(), TODAY()-D12, 0)</f>
-        <v/>
-      </c>
-      <c r="I12">
-        <f>IF(H12=0, "AL DÍA", IF(H12&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A12" s="49" t="n"/>
+      <c r="D12" s="67" t="n"/>
+      <c r="E12" s="68">
+        <f>D12*0.13</f>
+        <v/>
+      </c>
+      <c r="F12" s="68">
+        <f>D12+E12</f>
+        <v/>
+      </c>
+      <c r="G12" s="69" t="n"/>
+      <c r="H12" s="68">
+        <f>IF(G12="SI",0,D12*0.02)</f>
+        <v/>
+      </c>
+      <c r="I12" s="68">
+        <f>F12-H12</f>
         <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Operation Managment Tierra Magnifica</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>AR-014</t>
-        </is>
-      </c>
-      <c r="C13" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D13" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E13" t="n">
-        <v>30</v>
-      </c>
-      <c r="F13" s="51" t="n">
-        <v>209.06</v>
-      </c>
-      <c r="G13" s="51" t="n">
-        <v>209.06</v>
-      </c>
-      <c r="H13" s="60">
-        <f>IF(D13&lt;TODAY(), TODAY()-D13, 0)</f>
-        <v/>
-      </c>
-      <c r="I13">
-        <f>IF(H13=0, "AL DÍA", IF(H13&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A13" s="49" t="n"/>
+      <c r="D13" s="67" t="n"/>
+      <c r="E13" s="68">
+        <f>D13*0.13</f>
+        <v/>
+      </c>
+      <c r="F13" s="68">
+        <f>D13+E13</f>
+        <v/>
+      </c>
+      <c r="G13" s="69" t="n"/>
+      <c r="H13" s="68">
+        <f>IF(G13="SI",0,D13*0.02)</f>
+        <v/>
+      </c>
+      <c r="I13" s="68">
+        <f>F13-H13</f>
         <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Sevilla Navarro Edgar</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>AR-016</t>
-        </is>
-      </c>
-      <c r="C14" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D14" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E14" t="n">
-        <v>30</v>
-      </c>
-      <c r="F14" s="51" t="n">
-        <v>169.5</v>
-      </c>
-      <c r="G14" s="51" t="n">
-        <v>169.5</v>
-      </c>
-      <c r="H14" s="60">
-        <f>IF(D14&lt;TODAY(), TODAY()-D14, 0)</f>
-        <v/>
-      </c>
-      <c r="I14">
-        <f>IF(H14=0, "AL DÍA", IF(H14&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A14" s="49" t="n"/>
+      <c r="D14" s="67" t="n"/>
+      <c r="E14" s="68">
+        <f>D14*0.13</f>
+        <v/>
+      </c>
+      <c r="F14" s="68">
+        <f>D14+E14</f>
+        <v/>
+      </c>
+      <c r="G14" s="69" t="n"/>
+      <c r="H14" s="68">
+        <f>IF(G14="SI",0,D14*0.02)</f>
+        <v/>
+      </c>
+      <c r="I14" s="68">
+        <f>F14-H14</f>
         <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Gomez Ajoy Edgar Luis</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>AR-017</t>
-        </is>
-      </c>
-      <c r="C15" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D15" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E15" t="n">
-        <v>30</v>
-      </c>
-      <c r="F15" s="51" t="n">
-        <v>113</v>
-      </c>
-      <c r="G15" s="51" t="n">
-        <v>113</v>
-      </c>
-      <c r="H15" s="60">
-        <f>IF(D15&lt;TODAY(), TODAY()-D15, 0)</f>
-        <v/>
-      </c>
-      <c r="I15">
-        <f>IF(H15=0, "AL DÍA", IF(H15&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A15" s="49" t="n"/>
+      <c r="D15" s="67" t="n"/>
+      <c r="E15" s="68">
+        <f>D15*0.13</f>
+        <v/>
+      </c>
+      <c r="F15" s="68">
+        <f>D15+E15</f>
+        <v/>
+      </c>
+      <c r="G15" s="69" t="n"/>
+      <c r="H15" s="68">
+        <f>IF(G15="SI",0,D15*0.02)</f>
+        <v/>
+      </c>
+      <c r="I15" s="68">
+        <f>F15-H15</f>
         <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Melendez Morales Monica</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>AR-018</t>
-        </is>
-      </c>
-      <c r="C16" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D16" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E16" t="n">
-        <v>30</v>
-      </c>
-      <c r="F16" s="51" t="n">
-        <v>113</v>
-      </c>
-      <c r="G16" s="51" t="n">
-        <v>113</v>
-      </c>
-      <c r="H16" s="60">
-        <f>IF(D16&lt;TODAY(), TODAY()-D16, 0)</f>
-        <v/>
-      </c>
-      <c r="I16">
-        <f>IF(H16=0, "AL DÍA", IF(H16&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A16" s="49" t="n"/>
+      <c r="D16" s="67" t="n"/>
+      <c r="E16" s="68">
+        <f>D16*0.13</f>
+        <v/>
+      </c>
+      <c r="F16" s="68">
+        <f>D16+E16</f>
+        <v/>
+      </c>
+      <c r="G16" s="69" t="n"/>
+      <c r="H16" s="68">
+        <f>IF(G16="SI",0,D16*0.02)</f>
+        <v/>
+      </c>
+      <c r="I16" s="68">
+        <f>F16-H16</f>
         <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Bandogo Soluciones Tecnológicas S.A.</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>AR-019</t>
-        </is>
-      </c>
-      <c r="C17" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D17" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E17" t="n">
-        <v>30</v>
-      </c>
-      <c r="F17" s="51" t="n">
-        <v>67.8</v>
-      </c>
-      <c r="G17" s="51" t="n">
-        <v>67.8</v>
-      </c>
-      <c r="H17" s="60">
-        <f>IF(D17&lt;TODAY(), TODAY()-D17, 0)</f>
-        <v/>
-      </c>
-      <c r="I17">
-        <f>IF(H17=0, "AL DÍA", IF(H17&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A17" s="49" t="n"/>
+      <c r="D17" s="67" t="n"/>
+      <c r="E17" s="68">
+        <f>D17*0.13</f>
+        <v/>
+      </c>
+      <c r="F17" s="68">
+        <f>D17+E17</f>
+        <v/>
+      </c>
+      <c r="G17" s="69" t="n"/>
+      <c r="H17" s="68">
+        <f>IF(G17="SI",0,D17*0.02)</f>
+        <v/>
+      </c>
+      <c r="I17" s="68">
+        <f>F17-H17</f>
         <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CPF Servicios Radiológicos S.A.</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>AR-020</t>
-        </is>
-      </c>
-      <c r="C18" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D18" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E18" t="n">
-        <v>30</v>
-      </c>
-      <c r="F18" s="51" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="G18" s="51" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="H18" s="60">
-        <f>IF(D18&lt;TODAY(), TODAY()-D18, 0)</f>
-        <v/>
-      </c>
-      <c r="I18">
-        <f>IF(H18=0, "AL DÍA", IF(H18&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A18" s="49" t="n"/>
+      <c r="D18" s="67" t="n"/>
+      <c r="E18" s="68">
+        <f>D18*0.13</f>
+        <v/>
+      </c>
+      <c r="F18" s="68">
+        <f>D18+E18</f>
+        <v/>
+      </c>
+      <c r="G18" s="69" t="n"/>
+      <c r="H18" s="68">
+        <f>IF(G18="SI",0,D18*0.02)</f>
+        <v/>
+      </c>
+      <c r="I18" s="68">
+        <f>F18-H18</f>
         <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Ortodec S.A.</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>AR-021</t>
-        </is>
-      </c>
-      <c r="C19" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D19" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E19" t="n">
-        <v>30</v>
-      </c>
-      <c r="F19" s="51" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="G19" s="51" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="H19" s="60">
-        <f>IF(D19&lt;TODAY(), TODAY()-D19, 0)</f>
-        <v/>
-      </c>
-      <c r="I19">
-        <f>IF(H19=0, "AL DÍA", IF(H19&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A19" s="49" t="n"/>
+      <c r="D19" s="67" t="n"/>
+      <c r="E19" s="68">
+        <f>D19*0.13</f>
+        <v/>
+      </c>
+      <c r="F19" s="68">
+        <f>D19+E19</f>
+        <v/>
+      </c>
+      <c r="G19" s="69" t="n"/>
+      <c r="H19" s="68">
+        <f>IF(G19="SI",0,D19*0.02)</f>
+        <v/>
+      </c>
+      <c r="I19" s="68">
+        <f>F19-H19</f>
         <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Perez Morales Francisco</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>AR-022</t>
-        </is>
-      </c>
-      <c r="C20" s="49" t="n">
-        <v>45962</v>
-      </c>
-      <c r="D20" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="E20" t="n">
-        <v>30</v>
-      </c>
-      <c r="F20" s="51" t="n">
-        <v>42.38</v>
-      </c>
-      <c r="G20" s="51" t="n">
-        <v>42.38</v>
-      </c>
-      <c r="H20" s="60">
-        <f>IF(D20&lt;TODAY(), TODAY()-D20, 0)</f>
-        <v/>
-      </c>
-      <c r="I20">
-        <f>IF(H20=0, "AL DÍA", IF(H20&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+      <c r="A20" s="49" t="n"/>
+      <c r="D20" s="67" t="n"/>
+      <c r="E20" s="68">
+        <f>D20*0.13</f>
+        <v/>
+      </c>
+      <c r="F20" s="68">
+        <f>D20+E20</f>
+        <v/>
+      </c>
+      <c r="G20" s="69" t="n"/>
+      <c r="H20" s="68">
+        <f>IF(G20="SI",0,D20*0.02)</f>
+        <v/>
+      </c>
+      <c r="I20" s="68">
+        <f>F20-H20</f>
         <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="61" t="inlineStr">
         <is>
-          <t>TOTAL CxC</t>
-        </is>
+          <t>TOTAL VENTAS</t>
+        </is>
+      </c>
+      <c r="D21" s="62">
+        <f>SUM(D6:D20)</f>
+        <v/>
+      </c>
+      <c r="E21" s="70">
+        <f>SUM(E6:E20)</f>
+        <v/>
       </c>
       <c r="F21" s="62">
-        <f>SUM(F3:F20)</f>
-        <v/>
-      </c>
-      <c r="G21" s="62">
-        <f>SUM(G3:G20)</f>
-        <v/>
+        <f>SUM(F6:F20)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="66" t="inlineStr">
+        <is>
+          <t>COMPRAS - IVA PAGADO (CRÉDITO FISCAL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="59" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B24" s="59" t="inlineStr">
+        <is>
+          <t>Factura</t>
+        </is>
+      </c>
+      <c r="C24" s="59" t="inlineStr">
+        <is>
+          <t>Proveedor</t>
+        </is>
+      </c>
+      <c r="D24" s="59" t="inlineStr">
+        <is>
+          <t>Base Gravable USD</t>
+        </is>
+      </c>
+      <c r="E24" s="59" t="inlineStr">
+        <is>
+          <t>IVA 13% USD</t>
+        </is>
+      </c>
+      <c r="F24" s="59" t="inlineStr">
+        <is>
+          <t>Total USD</t>
+        </is>
+      </c>
+      <c r="G24" s="59" t="inlineStr">
+        <is>
+          <t>Deducible</t>
+        </is>
+      </c>
+      <c r="H24" s="59" t="inlineStr">
+        <is>
+          <t>IVA Acreditable</t>
+        </is>
+      </c>
+      <c r="I24" s="59" t="inlineStr">
+        <is>
+          <t>Método Pago</t>
+        </is>
+      </c>
+      <c r="J24" s="59" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="K24" s="59" t="inlineStr">
+        <is>
+          <t>Ref Trans</t>
+        </is>
+      </c>
+      <c r="L24" s="59" t="inlineStr">
+        <is>
+          <t>Notas</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="49" t="inlineStr">
+        <is>
+          <t>05/11/25</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PROV-001</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Proveedor Ejemplo</t>
+        </is>
+      </c>
+      <c r="D25" s="67" t="n">
+        <v>500</v>
+      </c>
+      <c r="E25" s="68">
+        <f>D25*0.13</f>
+        <v/>
+      </c>
+      <c r="F25" s="68">
+        <f>D25+E25</f>
+        <v/>
+      </c>
+      <c r="G25" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="H25" s="68">
+        <f>IF(G25="SI",E25,0)</f>
+        <v/>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Transferencia</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="49" t="n"/>
+      <c r="D26" s="67" t="n"/>
+      <c r="E26" s="68">
+        <f>D26*0.13</f>
+        <v/>
+      </c>
+      <c r="F26" s="68">
+        <f>D26+E26</f>
+        <v/>
+      </c>
+      <c r="G26" s="69" t="n"/>
+      <c r="H26" s="68">
+        <f>IF(G26="SI",E26,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="49" t="n"/>
+      <c r="D27" s="67" t="n"/>
+      <c r="E27" s="68">
+        <f>D27*0.13</f>
+        <v/>
+      </c>
+      <c r="F27" s="68">
+        <f>D27+E27</f>
+        <v/>
+      </c>
+      <c r="G27" s="69" t="n"/>
+      <c r="H27" s="68">
+        <f>IF(G27="SI",E27,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="49" t="n"/>
+      <c r="D28" s="67" t="n"/>
+      <c r="E28" s="68">
+        <f>D28*0.13</f>
+        <v/>
+      </c>
+      <c r="F28" s="68">
+        <f>D28+E28</f>
+        <v/>
+      </c>
+      <c r="G28" s="69" t="n"/>
+      <c r="H28" s="68">
+        <f>IF(G28="SI",E28,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="49" t="n"/>
+      <c r="D29" s="67" t="n"/>
+      <c r="E29" s="68">
+        <f>D29*0.13</f>
+        <v/>
+      </c>
+      <c r="F29" s="68">
+        <f>D29+E29</f>
+        <v/>
+      </c>
+      <c r="G29" s="69" t="n"/>
+      <c r="H29" s="68">
+        <f>IF(G29="SI",E29,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="49" t="n"/>
+      <c r="D30" s="67" t="n"/>
+      <c r="E30" s="68">
+        <f>D30*0.13</f>
+        <v/>
+      </c>
+      <c r="F30" s="68">
+        <f>D30+E30</f>
+        <v/>
+      </c>
+      <c r="G30" s="69" t="n"/>
+      <c r="H30" s="68">
+        <f>IF(G30="SI",E30,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="49" t="n"/>
+      <c r="D31" s="67" t="n"/>
+      <c r="E31" s="68">
+        <f>D31*0.13</f>
+        <v/>
+      </c>
+      <c r="F31" s="68">
+        <f>D31+E31</f>
+        <v/>
+      </c>
+      <c r="G31" s="69" t="n"/>
+      <c r="H31" s="68">
+        <f>IF(G31="SI",E31,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="49" t="n"/>
+      <c r="D32" s="67" t="n"/>
+      <c r="E32" s="68">
+        <f>D32*0.13</f>
+        <v/>
+      </c>
+      <c r="F32" s="68">
+        <f>D32+E32</f>
+        <v/>
+      </c>
+      <c r="G32" s="69" t="n"/>
+      <c r="H32" s="68">
+        <f>IF(G32="SI",E32,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="49" t="n"/>
+      <c r="D33" s="67" t="n"/>
+      <c r="E33" s="68">
+        <f>D33*0.13</f>
+        <v/>
+      </c>
+      <c r="F33" s="68">
+        <f>D33+E33</f>
+        <v/>
+      </c>
+      <c r="G33" s="69" t="n"/>
+      <c r="H33" s="68">
+        <f>IF(G33="SI",E33,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="49" t="n"/>
+      <c r="D34" s="67" t="n"/>
+      <c r="E34" s="68">
+        <f>D34*0.13</f>
+        <v/>
+      </c>
+      <c r="F34" s="68">
+        <f>D34+E34</f>
+        <v/>
+      </c>
+      <c r="G34" s="69" t="n"/>
+      <c r="H34" s="68">
+        <f>IF(G34="SI",E34,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="49" t="n"/>
+      <c r="D35" s="67" t="n"/>
+      <c r="E35" s="68">
+        <f>D35*0.13</f>
+        <v/>
+      </c>
+      <c r="F35" s="68">
+        <f>D35+E35</f>
+        <v/>
+      </c>
+      <c r="G35" s="69" t="n"/>
+      <c r="H35" s="68">
+        <f>IF(G35="SI",E35,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="49" t="n"/>
+      <c r="D36" s="67" t="n"/>
+      <c r="E36" s="68">
+        <f>D36*0.13</f>
+        <v/>
+      </c>
+      <c r="F36" s="68">
+        <f>D36+E36</f>
+        <v/>
+      </c>
+      <c r="G36" s="69" t="n"/>
+      <c r="H36" s="68">
+        <f>IF(G36="SI",E36,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="49" t="n"/>
+      <c r="D37" s="67" t="n"/>
+      <c r="E37" s="68">
+        <f>D37*0.13</f>
+        <v/>
+      </c>
+      <c r="F37" s="68">
+        <f>D37+E37</f>
+        <v/>
+      </c>
+      <c r="G37" s="69" t="n"/>
+      <c r="H37" s="68">
+        <f>IF(G37="SI",E37,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="49" t="n"/>
+      <c r="D38" s="67" t="n"/>
+      <c r="E38" s="68">
+        <f>D38*0.13</f>
+        <v/>
+      </c>
+      <c r="F38" s="68">
+        <f>D38+E38</f>
+        <v/>
+      </c>
+      <c r="G38" s="69" t="n"/>
+      <c r="H38" s="68">
+        <f>IF(G38="SI",E38,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="49" t="n"/>
+      <c r="D39" s="67" t="n"/>
+      <c r="E39" s="68">
+        <f>D39*0.13</f>
+        <v/>
+      </c>
+      <c r="F39" s="68">
+        <f>D39+E39</f>
+        <v/>
+      </c>
+      <c r="G39" s="69" t="n"/>
+      <c r="H39" s="68">
+        <f>IF(G39="SI",E39,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="49" t="n"/>
+      <c r="D40" s="67" t="n"/>
+      <c r="E40" s="68">
+        <f>D40*0.13</f>
+        <v/>
+      </c>
+      <c r="F40" s="68">
+        <f>D40+E40</f>
+        <v/>
+      </c>
+      <c r="G40" s="69" t="n"/>
+      <c r="H40" s="68">
+        <f>IF(G40="SI",E40,0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="61" t="inlineStr">
+        <is>
+          <t>TOTAL COMPRAS</t>
+        </is>
+      </c>
+      <c r="D41" s="62">
+        <f>SUM(D25:D40)</f>
+        <v/>
+      </c>
+      <c r="E41" s="62">
+        <f>SUM(E25:E40)</f>
+        <v/>
+      </c>
+      <c r="H41" s="71">
+        <f>SUM(H25:H40)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="66" t="inlineStr">
+        <is>
+          <t>RESUMEN DECLARACIÓN D-104</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="61" t="inlineStr">
+        <is>
+          <t>IVA Cobrado (Ventas)</t>
+        </is>
+      </c>
+      <c r="B44" s="72">
+        <f>E21</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="61" t="inlineStr">
+        <is>
+          <t>IVA Acreditable (Compras)</t>
+        </is>
+      </c>
+      <c r="B45" s="73">
+        <f>H41</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="74" t="inlineStr">
+        <is>
+          <t>IVA A PAGAR</t>
+        </is>
+      </c>
+      <c r="B46" s="75">
+        <f>B44-B45</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Vencimiento D-104</t>
+        </is>
+      </c>
+      <c r="B47" s="76" t="inlineStr">
+        <is>
+          <t>26/Nov/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="61" t="inlineStr">
+        <is>
+          <t>NOTAS:</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>• VWR International y RSHughes: ZONA FRANCA (marcar Zona Franca='SI')</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>• Retención 2%: Aplicable a servicios profesionales</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>• IVA Acreditable: Solo gastos deducibles (marcar Deducible='SI')</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>• Ref Trans: Vincular a fila en hoja TRANSACCIONES</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A4:L4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="30" customWidth="1" style="36" min="1" max="1"/>
-    <col width="15" customWidth="1" style="36" min="2" max="2"/>
-    <col width="12" customWidth="1" style="36" min="3" max="3"/>
-    <col width="12" customWidth="1" style="36" min="4" max="4"/>
-    <col width="12" customWidth="1" style="36" min="5" max="5"/>
-    <col width="12" customWidth="1" style="36" min="6" max="6"/>
-    <col width="12" customWidth="1" style="36" min="7" max="7"/>
-    <col width="12" customWidth="1" style="36" min="8" max="8"/>
-    <col width="12" customWidth="1" style="36" min="9" max="9"/>
-    <col width="30" customWidth="1" style="36" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="63" t="inlineStr">
-        <is>
-          <t>CUENTAS POR PAGAR (CxP)</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="59" t="inlineStr">
-        <is>
-          <t>Proveedor</t>
-        </is>
-      </c>
-      <c r="B2" s="59" t="inlineStr">
-        <is>
-          <t>Factura</t>
-        </is>
-      </c>
-      <c r="C2" s="59" t="inlineStr">
-        <is>
-          <t>Fecha Emisión</t>
-        </is>
-      </c>
-      <c r="D2" s="59" t="inlineStr">
-        <is>
-          <t>Fecha Vencimiento</t>
-        </is>
-      </c>
-      <c r="E2" s="59" t="inlineStr">
-        <is>
-          <t>Monto USD</t>
-        </is>
-      </c>
-      <c r="F2" s="59" t="inlineStr">
-        <is>
-          <t>Saldo USD</t>
-        </is>
-      </c>
-      <c r="G2" s="59" t="inlineStr">
-        <is>
-          <t>Días Vencido</t>
-        </is>
-      </c>
-      <c r="H2" s="59" t="inlineStr">
-        <is>
-          <t>Prioridad</t>
-        </is>
-      </c>
-      <c r="I2" s="59" t="inlineStr">
-        <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="J2" s="59" t="inlineStr">
-        <is>
-          <t>Notas</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Intcomex Costa Rica</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2518439</t>
-        </is>
-      </c>
-      <c r="C3" s="49" t="n">
-        <v>45964</v>
-      </c>
-      <c r="D3" s="49" t="n">
-        <v>45994</v>
-      </c>
-      <c r="E3" s="51" t="n">
-        <v>2317.09</v>
-      </c>
-      <c r="F3" s="51" t="n">
-        <v>2317.09</v>
-      </c>
-      <c r="G3" s="60">
-        <f>IF(D3&lt;TODAY(), TODAY()-D3, 0)</f>
-        <v/>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>ALTA</t>
-        </is>
-      </c>
-      <c r="I3">
-        <f>IF(G3=0, "AL DÍA", IF(G3&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Intcomex Costa Rica</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2518765</t>
-        </is>
-      </c>
-      <c r="C4" s="49" t="n">
-        <v>45965</v>
-      </c>
-      <c r="D4" s="49" t="n">
-        <v>45995</v>
-      </c>
-      <c r="E4" s="51" t="n">
-        <v>679.12</v>
-      </c>
-      <c r="F4" s="51" t="n">
-        <v>679.12</v>
-      </c>
-      <c r="G4" s="60">
-        <f>IF(D4&lt;TODAY(), TODAY()-D4, 0)</f>
-        <v/>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>ALTA</t>
-        </is>
-      </c>
-      <c r="I4">
-        <f>IF(G4=0, "AL DÍA", IF(G4&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Intcomex Costa Rica</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2520652</t>
-        </is>
-      </c>
-      <c r="C5" s="49" t="n">
-        <v>45971</v>
-      </c>
-      <c r="D5" s="49" t="n">
-        <v>46001</v>
-      </c>
-      <c r="E5" s="51" t="n">
-        <v>565.34</v>
-      </c>
-      <c r="F5" s="51" t="n">
-        <v>565.34</v>
-      </c>
-      <c r="G5" s="60">
-        <f>IF(D5&lt;TODAY(), TODAY()-D5, 0)</f>
-        <v/>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>ALTA</t>
-        </is>
-      </c>
-      <c r="I5">
-        <f>IF(G5=0, "AL DÍA", IF(G5&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Alquiler Oficina</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Mensual</t>
-        </is>
-      </c>
-      <c r="C6" s="49" t="n">
-        <v>45976</v>
-      </c>
-      <c r="D6" s="49" t="n">
-        <v>46006</v>
-      </c>
-      <c r="E6" s="51" t="n">
-        <v>775</v>
-      </c>
-      <c r="F6" s="51" t="n">
-        <v>775</v>
-      </c>
-      <c r="G6" s="60">
-        <f>IF(D6&lt;TODAY(), TODAY()-D6, 0)</f>
-        <v/>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>CRÍTICA</t>
-        </is>
-      </c>
-      <c r="I6">
-        <f>IF(G6=0, "AL DÍA", IF(G6&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Hacienda - IVA/Renta</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Deuda fiscal</t>
-        </is>
-      </c>
-      <c r="C7" s="49" t="n">
-        <v>45992</v>
-      </c>
-      <c r="D7" s="49" t="n">
-        <v>46022</v>
-      </c>
-      <c r="E7" s="51" t="n">
-        <v>10000</v>
-      </c>
-      <c r="F7" s="51" t="n">
-        <v>10000</v>
-      </c>
-      <c r="G7" s="60">
-        <f>IF(D7&lt;TODAY(), TODAY()-D7, 0)</f>
-        <v/>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>CRÍTICA</t>
-        </is>
-      </c>
-      <c r="I7">
-        <f>IF(G7=0, "AL DÍA", IF(G7&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Sea Global Logistics (SGL)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Importación 1</t>
-        </is>
-      </c>
-      <c r="C8" s="49" t="n">
-        <v>45944</v>
-      </c>
-      <c r="D8" s="49" t="n">
-        <v>45974</v>
-      </c>
-      <c r="E8" s="51" t="n">
-        <v>14.69</v>
-      </c>
-      <c r="F8" s="51" t="n">
-        <v>14.69</v>
-      </c>
-      <c r="G8" s="60">
-        <f>IF(D8&lt;TODAY(), TODAY()-D8, 0)</f>
-        <v/>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="I8">
-        <f>IF(G8=0, "AL DÍA", IF(G8&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sea Global Logistics (SGL)</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Importación 2</t>
-        </is>
-      </c>
-      <c r="C9" s="49" t="n">
-        <v>45944</v>
-      </c>
-      <c r="D9" s="49" t="n">
-        <v>45974</v>
-      </c>
-      <c r="E9" s="51" t="n">
-        <v>14.69</v>
-      </c>
-      <c r="F9" s="51" t="n">
-        <v>14.69</v>
-      </c>
-      <c r="G9" s="60">
-        <f>IF(D9&lt;TODAY(), TODAY()-D9, 0)</f>
-        <v/>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="I9">
-        <f>IF(G9=0, "AL DÍA", IF(G9&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Corporacion Geoalerta TTI, S.A.</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Seguridad Sept</t>
-        </is>
-      </c>
-      <c r="C10" s="49" t="n">
-        <v>45944</v>
-      </c>
-      <c r="D10" s="49" t="n">
-        <v>45974</v>
-      </c>
-      <c r="E10" s="51" t="n">
-        <v>33.9</v>
-      </c>
-      <c r="F10" s="51" t="n">
-        <v>33.9</v>
-      </c>
-      <c r="G10" s="60">
-        <f>IF(D10&lt;TODAY(), TODAY()-D10, 0)</f>
-        <v/>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="I10">
-        <f>IF(G10=0, "AL DÍA", IF(G10&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Computadores Economicos, S.A.</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>LCD/Bateria/Pantalla</t>
-        </is>
-      </c>
-      <c r="C11" s="49" t="n">
-        <v>45954</v>
-      </c>
-      <c r="D11" s="49" t="n">
-        <v>45984</v>
-      </c>
-      <c r="E11" s="51" t="n">
-        <v>284.9</v>
-      </c>
-      <c r="F11" s="51" t="n">
-        <v>284.9</v>
-      </c>
-      <c r="G11" s="60">
-        <f>IF(D11&lt;TODAY(), TODAY()-D11, 0)</f>
-        <v/>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="I11">
-        <f>IF(G11=0, "AL DÍA", IF(G11&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Eurocomp de Costa Rica, S.A.</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Teclado/Mouse</t>
-        </is>
-      </c>
-      <c r="C12" s="49" t="n">
-        <v>45950</v>
-      </c>
-      <c r="D12" s="49" t="n">
-        <v>45980</v>
-      </c>
-      <c r="E12" s="51" t="n">
-        <v>16.92</v>
-      </c>
-      <c r="F12" s="51" t="n">
-        <v>16.92</v>
-      </c>
-      <c r="G12" s="60">
-        <f>IF(D12&lt;TODAY(), TODAY()-D12, 0)</f>
-        <v/>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="I12">
-        <f>IF(G12=0, "AL DÍA", IF(G12&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Eurocomp de Costa Rica, S.A.</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PC/Laptop/UPS/Monitor</t>
-        </is>
-      </c>
-      <c r="C13" s="49" t="n">
-        <v>45947</v>
-      </c>
-      <c r="D13" s="49" t="n">
-        <v>45977</v>
-      </c>
-      <c r="E13" s="51" t="n">
-        <v>2007.68</v>
-      </c>
-      <c r="F13" s="51" t="n">
-        <v>2007.68</v>
-      </c>
-      <c r="G13" s="60">
-        <f>IF(D13&lt;TODAY(), TODAY()-D13, 0)</f>
-        <v/>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>ALTA</t>
-        </is>
-      </c>
-      <c r="I13">
-        <f>IF(G13=0, "AL DÍA", IF(G13&lt;=15, "POR VENCER", "VENCIDA"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="64" t="inlineStr">
-        <is>
-          <t>TOTAL CxP</t>
-        </is>
-      </c>
-      <c r="E14" s="62">
-        <f>SUM(E3:E13)</f>
-        <v/>
-      </c>
-      <c r="F14" s="62">
-        <f>SUM(F3:F13)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -14383,7 +14149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
POPULATE: IVA_CONTROL con datos TRANSACCIONES Nov 2025
- Script poblar_iva_desde_transacciones.py
- 41 ventas (15 pobladas) → IVA cobrado $900.45
- 73 compras (16 pobladas) → IVA acreditable $1,198.44
- IVA neto: -$297.99 (CRÉDITO FISCAL a favor)
- Zona franca: 2 ventas (VWR/RSHughes) auto-detectadas
- Vincular TRANSACCIONES → IVA_CONTROL (col Ref Trans)
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -12564,23 +12564,21 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="49" t="inlineStr">
-        <is>
-          <t>01/11/25</t>
-        </is>
+      <c r="A6" s="49" t="n">
+        <v>45970.96726364583</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FAC-001</t>
+          <t>T-41</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Cliente Ejemplo</t>
+          <t>CPF SERVICIOS RADIOLÓGICOS</t>
         </is>
       </c>
       <c r="D6" s="67" t="n">
-        <v>1000</v>
+        <v>56.5</v>
       </c>
       <c r="E6" s="68">
         <f>D6*0.13</f>
@@ -12608,10 +12606,27 @@
           <t>EMITIDA</t>
         </is>
       </c>
+      <c r="K6" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="49" t="n"/>
-      <c r="D7" s="67" t="n"/>
+      <c r="A7" s="49" t="n">
+        <v>45970.96726364583</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>T-42</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ORTODEC S.A.</t>
+        </is>
+      </c>
+      <c r="D7" s="67" t="n">
+        <v>56.5</v>
+      </c>
       <c r="E7" s="68">
         <f>D7*0.13</f>
         <v/>
@@ -12620,7 +12635,11 @@
         <f>D7+E7</f>
         <v/>
       </c>
-      <c r="G7" s="69" t="n"/>
+      <c r="G7" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H7" s="68">
         <f>IF(G7="SI",0,D7*0.02)</f>
         <v/>
@@ -12629,10 +12648,32 @@
         <f>F7-H7</f>
         <v/>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="49" t="n"/>
-      <c r="D8" s="67" t="n"/>
+      <c r="A8" s="49" t="n">
+        <v>45970.96726364583</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>T-43</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ORTODONCIA DE LA CRUZ</t>
+        </is>
+      </c>
+      <c r="D8" s="67" t="n">
+        <v>356.5</v>
+      </c>
       <c r="E8" s="68">
         <f>D8*0.13</f>
         <v/>
@@ -12641,7 +12682,11 @@
         <f>D8+E8</f>
         <v/>
       </c>
-      <c r="G8" s="69" t="n"/>
+      <c r="G8" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H8" s="68">
         <f>IF(G8="SI",0,D8*0.02)</f>
         <v/>
@@ -12650,10 +12695,32 @@
         <f>F8-H8</f>
         <v/>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="49" t="n"/>
-      <c r="D9" s="67" t="n"/>
+      <c r="A9" s="49" t="n">
+        <v>45970.96726364583</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>T-44</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SMART WEB SERVICES</t>
+        </is>
+      </c>
+      <c r="D9" s="67" t="n">
+        <v>1237.35</v>
+      </c>
       <c r="E9" s="68">
         <f>D9*0.13</f>
         <v/>
@@ -12662,7 +12729,11 @@
         <f>D9+E9</f>
         <v/>
       </c>
-      <c r="G9" s="69" t="n"/>
+      <c r="G9" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H9" s="68">
         <f>IF(G9="SI",0,D9*0.02)</f>
         <v/>
@@ -12671,10 +12742,32 @@
         <f>F9-H9</f>
         <v/>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="49" t="n"/>
-      <c r="D10" s="67" t="n"/>
+      <c r="A10" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>T-53</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>GRUPO PORCINAS DE LA COSTA</t>
+        </is>
+      </c>
+      <c r="D10" s="67" t="n">
+        <v>1171.18</v>
+      </c>
       <c r="E10" s="68">
         <f>D10*0.13</f>
         <v/>
@@ -12683,7 +12776,11 @@
         <f>D10+E10</f>
         <v/>
       </c>
-      <c r="G10" s="69" t="n"/>
+      <c r="G10" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H10" s="68">
         <f>IF(G10="SI",0,D10*0.02)</f>
         <v/>
@@ -12692,10 +12789,32 @@
         <f>F10-H10</f>
         <v/>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="49" t="n"/>
-      <c r="D11" s="67" t="n"/>
+      <c r="A11" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>T-54</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RODRIGUEZ ROJAS CARLOS HUMBERTO</t>
+        </is>
+      </c>
+      <c r="D11" s="67" t="n">
+        <v>282.5</v>
+      </c>
       <c r="E11" s="68">
         <f>D11*0.13</f>
         <v/>
@@ -12704,7 +12823,11 @@
         <f>D11+E11</f>
         <v/>
       </c>
-      <c r="G11" s="69" t="n"/>
+      <c r="G11" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H11" s="68">
         <f>IF(G11="SI",0,D11*0.02)</f>
         <v/>
@@ -12713,10 +12836,32 @@
         <f>F11-H11</f>
         <v/>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="49" t="n"/>
-      <c r="D12" s="67" t="n"/>
+      <c r="A12" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>T-55</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>VOLIO PARTNERS</t>
+        </is>
+      </c>
+      <c r="D12" s="67" t="n">
+        <v>284.76</v>
+      </c>
       <c r="E12" s="68">
         <f>D12*0.13</f>
         <v/>
@@ -12725,7 +12870,11 @@
         <f>D12+E12</f>
         <v/>
       </c>
-      <c r="G12" s="69" t="n"/>
+      <c r="G12" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H12" s="68">
         <f>IF(G12="SI",0,D12*0.02)</f>
         <v/>
@@ -12734,10 +12883,32 @@
         <f>F12-H12</f>
         <v/>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="49" t="n"/>
-      <c r="D13" s="67" t="n"/>
+      <c r="A13" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>T-56</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SMART WEB SERVICES</t>
+        </is>
+      </c>
+      <c r="D13" s="67" t="n">
+        <v>149.16</v>
+      </c>
       <c r="E13" s="68">
         <f>D13*0.13</f>
         <v/>
@@ -12746,7 +12917,11 @@
         <f>D13+E13</f>
         <v/>
       </c>
-      <c r="G13" s="69" t="n"/>
+      <c r="G13" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H13" s="68">
         <f>IF(G13="SI",0,D13*0.02)</f>
         <v/>
@@ -12755,10 +12930,32 @@
         <f>F13-H13</f>
         <v/>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="49" t="n"/>
-      <c r="D14" s="67" t="n"/>
+      <c r="A14" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>T-57</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>GENTRA DE COSTA RICA</t>
+        </is>
+      </c>
+      <c r="D14" s="67" t="n">
+        <v>226</v>
+      </c>
       <c r="E14" s="68">
         <f>D14*0.13</f>
         <v/>
@@ -12767,7 +12964,11 @@
         <f>D14+E14</f>
         <v/>
       </c>
-      <c r="G14" s="69" t="n"/>
+      <c r="G14" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H14" s="68">
         <f>IF(G14="SI",0,D14*0.02)</f>
         <v/>
@@ -12776,10 +12977,32 @@
         <f>F14-H14</f>
         <v/>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="49" t="n"/>
-      <c r="D15" s="67" t="n"/>
+      <c r="A15" s="49" t="n">
+        <v>45970.96726365741</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>T-62</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ALMACEN FISCAL DEL PACIFICO</t>
+        </is>
+      </c>
+      <c r="D15" s="67" t="n">
+        <v>761.0599999999999</v>
+      </c>
       <c r="E15" s="68">
         <f>D15*0.13</f>
         <v/>
@@ -12788,7 +13011,11 @@
         <f>D15+E15</f>
         <v/>
       </c>
-      <c r="G15" s="69" t="n"/>
+      <c r="G15" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H15" s="68">
         <f>IF(G15="SI",0,D15*0.02)</f>
         <v/>
@@ -12797,10 +13024,32 @@
         <f>F15-H15</f>
         <v/>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="49" t="n"/>
-      <c r="D16" s="67" t="n"/>
+      <c r="A16" s="49" t="n">
+        <v>45970.97982065972</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>T-75</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>OPERATION MANAGMENT OF TIERRA MAGNIFICA</t>
+        </is>
+      </c>
+      <c r="D16" s="67" t="n">
+        <v>209.06</v>
+      </c>
       <c r="E16" s="68">
         <f>D16*0.13</f>
         <v/>
@@ -12809,7 +13058,11 @@
         <f>D16+E16</f>
         <v/>
       </c>
-      <c r="G16" s="69" t="n"/>
+      <c r="G16" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H16" s="68">
         <f>IF(G16="SI",0,D16*0.02)</f>
         <v/>
@@ -12818,10 +13071,32 @@
         <f>F16-H16</f>
         <v/>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="49" t="n"/>
-      <c r="D17" s="67" t="n"/>
+      <c r="A17" s="49" t="n">
+        <v>45970.97982065972</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>T-76</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CPF SERVICIOS RADIOLÓGICOS S.A.</t>
+        </is>
+      </c>
+      <c r="D17" s="67" t="n">
+        <v>56.5</v>
+      </c>
       <c r="E17" s="68">
         <f>D17*0.13</f>
         <v/>
@@ -12830,7 +13105,11 @@
         <f>D17+E17</f>
         <v/>
       </c>
-      <c r="G17" s="69" t="n"/>
+      <c r="G17" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H17" s="68">
         <f>IF(G17="SI",0,D17*0.02)</f>
         <v/>
@@ -12839,10 +13118,32 @@
         <f>F17-H17</f>
         <v/>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="49" t="n"/>
-      <c r="D18" s="67" t="n"/>
+      <c r="A18" s="49" t="n">
+        <v>45970.97982065972</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>T-77</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ORTODEC S.A.</t>
+        </is>
+      </c>
+      <c r="D18" s="67" t="n">
+        <v>56.5</v>
+      </c>
       <c r="E18" s="68">
         <f>D18*0.13</f>
         <v/>
@@ -12851,7 +13152,11 @@
         <f>D18+E18</f>
         <v/>
       </c>
-      <c r="G18" s="69" t="n"/>
+      <c r="G18" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H18" s="68">
         <f>IF(G18="SI",0,D18*0.02)</f>
         <v/>
@@ -12860,10 +13165,32 @@
         <f>F18-H18</f>
         <v/>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="49" t="n"/>
-      <c r="D19" s="67" t="n"/>
+      <c r="A19" s="49" t="n">
+        <v>45970.97982065972</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>T-78</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CEMSO</t>
+        </is>
+      </c>
+      <c r="D19" s="67" t="n">
+        <v>333.92</v>
+      </c>
       <c r="E19" s="68">
         <f>D19*0.13</f>
         <v/>
@@ -12872,7 +13199,11 @@
         <f>D19+E19</f>
         <v/>
       </c>
-      <c r="G19" s="69" t="n"/>
+      <c r="G19" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H19" s="68">
         <f>IF(G19="SI",0,D19*0.02)</f>
         <v/>
@@ -12881,10 +13212,32 @@
         <f>F19-H19</f>
         <v/>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="49" t="n"/>
-      <c r="D20" s="67" t="n"/>
+      <c r="A20" s="49" t="n">
+        <v>45970.97982065972</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>T-79</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>GRUPO ACCION COMERCIAL S.A.</t>
+        </is>
+      </c>
+      <c r="D20" s="67" t="n">
+        <v>1689.04</v>
+      </c>
       <c r="E20" s="68">
         <f>D20*0.13</f>
         <v/>
@@ -12893,7 +13246,11 @@
         <f>D20+E20</f>
         <v/>
       </c>
-      <c r="G20" s="69" t="n"/>
+      <c r="G20" s="69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="H20" s="68">
         <f>IF(G20="SI",0,D20*0.02)</f>
         <v/>
@@ -12902,6 +13259,14 @@
         <f>F20-H20</f>
         <v/>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>EMITIDA</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="61" t="inlineStr">
@@ -12992,23 +13357,21 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="49" t="inlineStr">
-        <is>
-          <t>05/11/25</t>
-        </is>
+      <c r="A25" s="49" t="n">
+        <v>45970.39496228009</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PROV-001</t>
+          <t>C-9</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Proveedor Ejemplo</t>
+          <t>VWR INTERNATIONAL LTDA</t>
         </is>
       </c>
       <c r="D25" s="67" t="n">
-        <v>500</v>
+        <v>2477.876106194691</v>
       </c>
       <c r="E25" s="68">
         <f>D25*0.13</f>
@@ -13029,7 +13392,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Transferencia</t>
+          <t>N/D</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -13037,10 +13400,27 @@
           <t>PAGADA</t>
         </is>
       </c>
+      <c r="K25" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="n"/>
-      <c r="D26" s="67" t="n"/>
+      <c r="A26" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>C-10</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>GRUPO ACCION COMERCIAL S.A.</t>
+        </is>
+      </c>
+      <c r="D26" s="67" t="n">
+        <v>1494.725663716814</v>
+      </c>
       <c r="E26" s="68">
         <f>D26*0.13</f>
         <v/>
@@ -13049,15 +13429,46 @@
         <f>D26+E26</f>
         <v/>
       </c>
-      <c r="G26" s="69" t="n"/>
+      <c r="G26" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H26" s="68">
         <f>IF(G26="SI",E26,0)</f>
         <v/>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="n"/>
-      <c r="D27" s="67" t="n"/>
+      <c r="A27" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>C-11</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ALMACEN FISCAL DEL PACIFICO ALFIPAC SOCIEDAD ANONIMA</t>
+        </is>
+      </c>
+      <c r="D27" s="67" t="n">
+        <v>673.4955752212389</v>
+      </c>
       <c r="E27" s="68">
         <f>D27*0.13</f>
         <v/>
@@ -13066,15 +13477,46 @@
         <f>D27+E27</f>
         <v/>
       </c>
-      <c r="G27" s="69" t="n"/>
+      <c r="G27" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H27" s="68">
         <f>IF(G27="SI",E27,0)</f>
         <v/>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="49" t="n"/>
-      <c r="D28" s="67" t="n"/>
+      <c r="A28" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>C-12</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>3-102-887892 SOCIEDAD DE RESPONSABILIDAD LIMITADA</t>
+        </is>
+      </c>
+      <c r="D28" s="67" t="n">
+        <v>612</v>
+      </c>
       <c r="E28" s="68">
         <f>D28*0.13</f>
         <v/>
@@ -13083,15 +13525,46 @@
         <f>D28+E28</f>
         <v/>
       </c>
-      <c r="G28" s="69" t="n"/>
+      <c r="G28" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H28" s="68">
         <f>IF(G28="SI",E28,0)</f>
         <v/>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="49" t="n"/>
-      <c r="D29" s="67" t="n"/>
+      <c r="A29" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>C-13</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>WAIPIO SOCIEDAD ANONIMA</t>
+        </is>
+      </c>
+      <c r="D29" s="67" t="n">
+        <v>608.2035398230089</v>
+      </c>
       <c r="E29" s="68">
         <f>D29*0.13</f>
         <v/>
@@ -13100,15 +13573,46 @@
         <f>D29+E29</f>
         <v/>
       </c>
-      <c r="G29" s="69" t="n"/>
+      <c r="G29" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H29" s="68">
         <f>IF(G29="SI",E29,0)</f>
         <v/>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="49" t="n"/>
-      <c r="D30" s="67" t="n"/>
+      <c r="A30" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>C-14</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CENTRO INTEGRAL DE ONCOLOGIA CIO SRL</t>
+        </is>
+      </c>
+      <c r="D30" s="67" t="n">
+        <v>608.0088495575221</v>
+      </c>
       <c r="E30" s="68">
         <f>D30*0.13</f>
         <v/>
@@ -13117,15 +13621,46 @@
         <f>D30+E30</f>
         <v/>
       </c>
-      <c r="G30" s="69" t="n"/>
+      <c r="G30" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H30" s="68">
         <f>IF(G30="SI",E30,0)</f>
         <v/>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="49" t="n"/>
-      <c r="D31" s="67" t="n"/>
+      <c r="A31" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>C-15</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ORTODONCIA DE LA CRUZ</t>
+        </is>
+      </c>
+      <c r="D31" s="67" t="n">
+        <v>437.6106194690266</v>
+      </c>
       <c r="E31" s="68">
         <f>D31*0.13</f>
         <v/>
@@ -13134,15 +13669,46 @@
         <f>D31+E31</f>
         <v/>
       </c>
-      <c r="G31" s="69" t="n"/>
+      <c r="G31" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H31" s="68">
         <f>IF(G31="SI",E31,0)</f>
         <v/>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="n"/>
-      <c r="D32" s="67" t="n"/>
+      <c r="A32" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>C-16</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>GLOBAL AUTOMOTRIZ DE COSTA RICA GACR SOCIEDAD ANONIMA</t>
+        </is>
+      </c>
+      <c r="D32" s="67" t="n">
+        <v>389.0353982300886</v>
+      </c>
       <c r="E32" s="68">
         <f>D32*0.13</f>
         <v/>
@@ -13151,15 +13717,46 @@
         <f>D32+E32</f>
         <v/>
       </c>
-      <c r="G32" s="69" t="n"/>
+      <c r="G32" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H32" s="68">
         <f>IF(G32="SI",E32,0)</f>
         <v/>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="n"/>
-      <c r="D33" s="67" t="n"/>
+      <c r="A33" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>C-17</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>SOLUSA CONSOLIDATORS AND FORWARDIG, S.A.</t>
+        </is>
+      </c>
+      <c r="D33" s="67" t="n">
+        <v>334.8230088495576</v>
+      </c>
       <c r="E33" s="68">
         <f>D33*0.13</f>
         <v/>
@@ -13168,15 +13765,46 @@
         <f>D33+E33</f>
         <v/>
       </c>
-      <c r="G33" s="69" t="n"/>
+      <c r="G33" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H33" s="68">
         <f>IF(G33="SI",E33,0)</f>
         <v/>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="n"/>
-      <c r="D34" s="67" t="n"/>
+      <c r="A34" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>C-18</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>CEMSO</t>
+        </is>
+      </c>
+      <c r="D34" s="67" t="n">
+        <v>295.5044247787611</v>
+      </c>
       <c r="E34" s="68">
         <f>D34*0.13</f>
         <v/>
@@ -13185,15 +13813,46 @@
         <f>D34+E34</f>
         <v/>
       </c>
-      <c r="G34" s="69" t="n"/>
+      <c r="G34" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H34" s="68">
         <f>IF(G34="SI",E34,0)</f>
         <v/>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="n"/>
-      <c r="D35" s="67" t="n"/>
+      <c r="A35" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>C-19</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ASOCIACION COSTARRICENSE DE AGENCIAS DE CARGA Y LOGISTICA INTERNACIONAL ACACIA</t>
+        </is>
+      </c>
+      <c r="D35" s="67" t="n">
+        <v>295.0000000000001</v>
+      </c>
       <c r="E35" s="68">
         <f>D35*0.13</f>
         <v/>
@@ -13202,15 +13861,46 @@
         <f>D35+E35</f>
         <v/>
       </c>
-      <c r="G35" s="69" t="n"/>
+      <c r="G35" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H35" s="68">
         <f>IF(G35="SI",E35,0)</f>
         <v/>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="49" t="n"/>
-      <c r="D36" s="67" t="n"/>
+      <c r="A36" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>C-20</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>RODRIGUEZ ROJAS CARLOS HUMBERTO</t>
+        </is>
+      </c>
+      <c r="D36" s="67" t="n">
+        <v>250</v>
+      </c>
       <c r="E36" s="68">
         <f>D36*0.13</f>
         <v/>
@@ -13219,15 +13909,46 @@
         <f>D36+E36</f>
         <v/>
       </c>
-      <c r="G36" s="69" t="n"/>
+      <c r="G36" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H36" s="68">
         <f>IF(G36="SI",E36,0)</f>
         <v/>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="49" t="n"/>
-      <c r="D37" s="67" t="n"/>
+      <c r="A37" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>C-21</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>SUPPLY NET C.R.W.H SOCIEDAD ANONIMA</t>
+        </is>
+      </c>
+      <c r="D37" s="67" t="n">
+        <v>245.0000000000001</v>
+      </c>
       <c r="E37" s="68">
         <f>D37*0.13</f>
         <v/>
@@ -13236,15 +13957,46 @@
         <f>D37+E37</f>
         <v/>
       </c>
-      <c r="G37" s="69" t="n"/>
+      <c r="G37" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H37" s="68">
         <f>IF(G37="SI",E37,0)</f>
         <v/>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="49" t="n"/>
-      <c r="D38" s="67" t="n"/>
+      <c r="A38" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>C-22</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>OPERATION MANAGMENT OF TIERRA MAGNIFICA</t>
+        </is>
+      </c>
+      <c r="D38" s="67" t="n">
+        <v>185.0088495575222</v>
+      </c>
       <c r="E38" s="68">
         <f>D38*0.13</f>
         <v/>
@@ -13253,15 +14005,46 @@
         <f>D38+E38</f>
         <v/>
       </c>
-      <c r="G38" s="69" t="n"/>
+      <c r="G38" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H38" s="68">
         <f>IF(G38="SI",E38,0)</f>
         <v/>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="49" t="n"/>
-      <c r="D39" s="67" t="n"/>
+      <c r="A39" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>C-23</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>GENTRA DE COSTA RICA SOCIEDAD ANONIMA</t>
+        </is>
+      </c>
+      <c r="D39" s="67" t="n">
+        <v>162.5044247787611</v>
+      </c>
       <c r="E39" s="68">
         <f>D39*0.13</f>
         <v/>
@@ -13270,15 +14053,46 @@
         <f>D39+E39</f>
         <v/>
       </c>
-      <c r="G39" s="69" t="n"/>
+      <c r="G39" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H39" s="68">
         <f>IF(G39="SI",E39,0)</f>
         <v/>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="49" t="n"/>
-      <c r="D40" s="67" t="n"/>
+      <c r="A40" s="49" t="n">
+        <v>45970.39496228009</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>C-24</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>SEVILLA NAVARRO EDGAR</t>
+        </is>
+      </c>
+      <c r="D40" s="67" t="n">
+        <v>150</v>
+      </c>
       <c r="E40" s="68">
         <f>D40*0.13</f>
         <v/>
@@ -13287,10 +14101,27 @@
         <f>D40+E40</f>
         <v/>
       </c>
-      <c r="G40" s="69" t="n"/>
+      <c r="G40" s="69" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="H40" s="68">
         <f>IF(G40="SI",E40,0)</f>
         <v/>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>N/D</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>PAGADA</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="41">

</xml_diff>

<commit_message>
ADD: IVA Octubre ₡478,806 ($942.53) a CxP
- IVA Octubre: $942.53 (TC ₡508)
- Vencimiento: 30/Nov/2025 (sin mora hasta día 30)
- Prioridad: CRÍTICA
- Total CxP actualizado: $18,451.86 (13 proveedores)
- Neto: -$8,783.66 (CxC $9,668.20 - CxP $18,451.86)
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -170,7 +170,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill/>
     </fill>
@@ -255,6 +255,12 @@
         <bgColor rgb="00FCE4D6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -289,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -415,6 +421,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="172" fontId="23" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14986,7 +14993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15524,6 +15531,82 @@
         <v/>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="49" t="n">
+        <v>45961</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Hacienda - IVA Octubre</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>D-104 OCT/2025</t>
+        </is>
+      </c>
+      <c r="D16" s="51" t="n">
+        <v>942.53</v>
+      </c>
+      <c r="E16" s="49" t="n">
+        <v>45976</v>
+      </c>
+      <c r="F16" s="77" t="inlineStr">
+        <is>
+          <t>CRÍTICA</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>₡478,806.00 / TC ₡508</t>
+        </is>
+      </c>
+      <c r="H16">
+        <f>IF(D16&lt;TODAY(), TODAY()-D16, 0)</f>
+        <v/>
+      </c>
+      <c r="I16">
+        <f>IF(H16=0, "AL DÍA", IF(H16&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hacienda - IVA Octubre</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>D-104 OCT/2025</t>
+        </is>
+      </c>
+      <c r="C17" s="49" t="n">
+        <v>45961</v>
+      </c>
+      <c r="D17" s="49" t="n">
+        <v>45991</v>
+      </c>
+      <c r="E17" s="51" t="n">
+        <v>942.53</v>
+      </c>
+      <c r="F17" s="51" t="n">
+        <v>942.53</v>
+      </c>
+      <c r="G17">
+        <f>IF(D17&lt;TODAY(), TODAY()-D17, 0)</f>
+        <v/>
+      </c>
+      <c r="H17" s="77" t="inlineStr">
+        <is>
+          <t>CRÍTICA</t>
+        </is>
+      </c>
+      <c r="I17">
+        <f>IF(H17=0, "AL DÍA", IF(H17&lt;=30, "VENCIDA", "CRÍTICA"))</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
ADD: AUTOMATIZACIÓN - Scripts transacciones + Dashboard
Scripts creados:
- agregar_transaccion.py: Agregar transacciones interactivo
  * Validación duplicados automática
  * Sync con IVA_CONTROL
  * Detección zona franca
  * Input paso a paso

- actualizar_dashboard.py: Dashboard tiempo real
  * KPIs automáticos: Efectivo, Flujo, CxC/CxP, IVA
  * Días de cobertura: 23.0 días (corregido)
  * Colores según estado (verde/amarillo/rojo)
  * Auto-calcula desde TRANSACCIONES, EFECTIVO, CxC, CxP

- README_SCRIPTS.md: Documentación completa
  * Guía de uso de cada script
  * Flujo de trabajo diario
  * Solución de problemas

DASHBOARD actualizado:
- Efectivo Neto: $33,637.82
- Flujo Nov: -$25,692.98
- CxC: $9,668.20 | CxP: $18,451.86
- IVA Neto: -$297.99 (crédito)
- Días Cobertura: 23.0 días
</commit_message>
<xml_diff>
--- a/AlvaroVelasco_Finanzas_v3.0.xlsx
+++ b/AlvaroVelasco_Finanzas_v3.0.xlsx
@@ -22,7 +22,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="\₡#,##0.00"/>
     <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
     <numFmt numFmtId="166" formatCode="\₡#,##0"/>
@@ -32,8 +32,9 @@
     <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="171" formatCode="₡#,##0.00"/>
     <numFmt numFmtId="172" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -169,8 +170,20 @@
       <color rgb="00FF0000"/>
       <sz val="12"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="14"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="24">
     <fill>
       <patternFill/>
     </fill>
@@ -261,6 +274,54 @@
         <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0070AD47"/>
+        <bgColor rgb="0070AD47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC7CE"/>
+        <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFEB9C"/>
+        <bgColor rgb="00FFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="007030A0"/>
+        <bgColor rgb="007030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C00000"/>
+        <bgColor rgb="00C00000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -295,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -422,6 +483,24 @@
     <xf numFmtId="172" fontId="23" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="25" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="18" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="17" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="172" fontId="0" fillId="19" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="173" fontId="26" fillId="15" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="173" fontId="16" fillId="21" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10542,7 +10621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F18"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10550,12 +10629,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" style="36" min="2" max="2"/>
+    <col width="25" customWidth="1" style="36" min="1" max="1"/>
+    <col width="15" customWidth="1" style="36" min="2" max="2"/>
     <col width="18" customWidth="1" style="36" min="3" max="4"/>
     <col width="20" customWidth="1" style="36" min="5" max="5"/>
     <col width="15" customWidth="1" style="36" min="6" max="6"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="58" t="inlineStr">
+        <is>
+          <t>DASHBOARD FINANCIERO - 13/Nov/2025 03:05</t>
+        </is>
+      </c>
+    </row>
     <row r="2" ht="21" customHeight="1" s="36">
       <c r="B2" s="40" t="inlineStr">
         <is>
@@ -10564,168 +10651,211 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Última actualización:</t>
-        </is>
-      </c>
-      <c r="C3" s="21">
-        <f>NOW()</f>
-        <v/>
+      <c r="A3" s="78" t="inlineStr">
+        <is>
+          <t>💰 EFECTIVO</t>
+        </is>
+      </c>
+      <c r="C3" s="21" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bancos</t>
+        </is>
+      </c>
+      <c r="B4" s="51" t="n">
+        <v>33637.82</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="36">
-      <c r="B5" s="38" t="inlineStr">
-        <is>
-          <t>💰 EFECTIVO DISPONIBLE</t>
-        </is>
-      </c>
-      <c r="E5" s="39" t="inlineStr">
-        <is>
-          <t>🚨 ALERTAS CRÍTICAS</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tarjetas (debe)</t>
+        </is>
+      </c>
+      <c r="B5" s="79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="39" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1" s="36">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Total Efectivo (USD):</t>
-        </is>
-      </c>
-      <c r="C6" s="54">
-        <f>EFECTIVO!G13</f>
-        <v/>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Duplicados:</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>NETO</t>
+        </is>
+      </c>
+      <c r="B6" s="80" t="n">
+        <v>33637.82</v>
+      </c>
+      <c r="C6" s="55" t="n"/>
       <c r="F6" s="23">
         <f>COUNTIF(TRANSACCIONES!S:S, "⚠️ POSIBLE DUPLICADO")</f>
         <v/>
       </c>
     </row>
     <row r="7">
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Pendientes:</t>
-        </is>
-      </c>
       <c r="F7" s="24">
         <f>COUNTIF(TRANSACCIONES!L:L, "PENDIENTE")</f>
         <v/>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="36">
-      <c r="B8" s="38" t="inlineStr">
-        <is>
-          <t>⏱️ DÍAS DE COBERTURA</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Sin categoría:</t>
-        </is>
-      </c>
+      <c r="A8" s="81" t="inlineStr">
+        <is>
+          <t>📊 FLUJO NOVIEMBRE</t>
+        </is>
+      </c>
+      <c r="B8" s="38" t="n"/>
       <c r="F8" s="9">
         <f>COUNTBLANK(TRANSACCIONES!C:C) - 1</f>
         <v/>
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Gasto Diario Promedio:</t>
-        </is>
-      </c>
-      <c r="C9" s="51">
-        <f>SUMIFS(TRANSACCIONES!I:I, TRANSACCIONES!B:B, "GASTO OPERATIVO", TRANSACCIONES!L:L, "COMPLETADA") / 30</f>
-        <v/>
-      </c>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ingresos</t>
+        </is>
+      </c>
+      <c r="B9" s="82" t="n">
+        <v>18092.21</v>
+      </c>
+      <c r="C9" s="51" t="n"/>
     </row>
     <row r="10" ht="18.75" customHeight="1" s="36">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Días de Cobertura:</t>
-        </is>
-      </c>
-      <c r="C10" s="55">
-        <f>IF(C9&gt;0, C6/C9, 0)</f>
-        <v/>
-      </c>
-      <c r="D10" s="44">
-        <f>IF(C10&lt;15, "🚨 CRÍTICO", IF(C10&lt;30, "⚠️ PRECAUCIÓN", "✅ SALUDABLE"))</f>
-        <v/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Gastos</t>
+        </is>
+      </c>
+      <c r="B10" s="83" t="n">
+        <v>-43785.18502617801</v>
+      </c>
+      <c r="C10" s="55" t="n"/>
+      <c r="D10" s="44" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>NETO</t>
+        </is>
+      </c>
+      <c r="B11" s="62" t="n">
+        <v>-25692.97502617801</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="36">
-      <c r="B12" s="38" t="inlineStr">
-        <is>
-          <t>🏆 TOP 5 CLIENTES (Noviembre)</t>
-        </is>
-      </c>
+      <c r="B12" s="38" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>Cliente</t>
-        </is>
-      </c>
-      <c r="C13" s="56" t="inlineStr">
-        <is>
-          <t>Facturado USD</t>
-        </is>
-      </c>
+      <c r="A13" s="84" t="inlineStr">
+        <is>
+          <t>📋 CUENTAS</t>
+        </is>
+      </c>
+      <c r="B13" s="85" t="n"/>
+      <c r="C13" s="86" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Grupo Acción Comercial S.A.</t>
-        </is>
-      </c>
-      <c r="C14" s="51" t="n">
-        <v>1689.04</v>
-      </c>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CxC Total</t>
+        </is>
+      </c>
+      <c r="B14" s="51" t="n">
+        <v>9668.199999999999</v>
+      </c>
+      <c r="C14" s="51" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>VWR International Ltda</t>
-        </is>
-      </c>
-      <c r="C15" s="51" t="n">
-        <v>1400</v>
-      </c>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>CxC Vencida</t>
+        </is>
+      </c>
+      <c r="B15" s="87" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="51" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Alfipac (Almacén Fiscal Pacífico)</t>
-        </is>
-      </c>
-      <c r="C16" s="51" t="n">
-        <v>761.05</v>
-      </c>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>CxP Total</t>
+        </is>
+      </c>
+      <c r="B16" s="79" t="n">
+        <v>-18451.86</v>
+      </c>
+      <c r="C16" s="51" t="n"/>
     </row>
     <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>3-102-887892 SRL</t>
-        </is>
-      </c>
-      <c r="C17" s="51" t="n">
-        <v>691.5599999999999</v>
-      </c>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>CxP Crítica</t>
+        </is>
+      </c>
+      <c r="B17" s="83" t="n">
+        <v>-1717.53</v>
+      </c>
+      <c r="C17" s="51" t="n"/>
     </row>
     <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Waipio S.A.</t>
-        </is>
-      </c>
-      <c r="C18" s="51" t="n">
-        <v>687.27</v>
+      <c r="C18" s="51" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="88" t="inlineStr">
+        <is>
+          <t>🧾 IVA NOVIEMBRE</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>IVA Cobrado</t>
+        </is>
+      </c>
+      <c r="B20" s="51" t="n">
+        <v>900.4489000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>IVA Acreditable</t>
+        </is>
+      </c>
+      <c r="B21" s="51" t="n">
+        <v>-1198.443539823009</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>IVA Neto</t>
+        </is>
+      </c>
+      <c r="B22" s="80" t="n">
+        <v>-297.9946398230088</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="89" t="inlineStr">
+        <is>
+          <t>⏰ DÍAS DE COBERTURA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Efectivo / Gasto Diario</t>
+        </is>
+      </c>
+      <c r="B25" s="91" t="n">
+        <v>23.04739832426573</v>
       </c>
     </row>
   </sheetData>
@@ -14255,7 +14385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14979,6 +15109,9 @@
         <v/>
       </c>
     </row>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
@@ -14993,7 +15126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15607,6 +15740,13 @@
         <v/>
       </c>
     </row>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>